<commit_message>
Updated test run status
</commit_message>
<xml_diff>
--- a/src/com/supplierconnection/xls/TestSuite1.xlsx
+++ b/src/com/supplierconnection/xls/TestSuite1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12315" windowHeight="2055" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12315" windowHeight="2055" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -3938,7 +3938,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="C4" sqref="C4:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3966,7 +3966,7 @@
         <v>50</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -3977,7 +3977,7 @@
         <v>52</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -3988,7 +3988,7 @@
         <v>63</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -3998,8 +3998,8 @@
       <c r="B5" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>29</v>
+      <c r="C5" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -4009,8 +4009,8 @@
       <c r="B6" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>29</v>
+      <c r="C6" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -4020,8 +4020,8 @@
       <c r="B7" t="s">
         <v>139</v>
       </c>
-      <c r="C7" t="s">
-        <v>29</v>
+      <c r="C7" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -4031,8 +4031,8 @@
       <c r="B8" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="C8" s="22" t="s">
-        <v>29</v>
+      <c r="C8" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -4042,8 +4042,8 @@
       <c r="B9" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C9" t="s">
-        <v>29</v>
+      <c r="C9" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -4053,8 +4053,8 @@
       <c r="B10" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C10" t="s">
-        <v>29</v>
+      <c r="C10" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -4064,8 +4064,8 @@
       <c r="B11" t="s">
         <v>306</v>
       </c>
-      <c r="C11" t="s">
-        <v>29</v>
+      <c r="C11" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -4075,7 +4075,7 @@
       <c r="B12" t="s">
         <v>332</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="7" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4086,8 +4086,8 @@
       <c r="B13" t="s">
         <v>68</v>
       </c>
-      <c r="C13" t="s">
-        <v>29</v>
+      <c r="C13" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -4097,8 +4097,8 @@
       <c r="B14" t="s">
         <v>335</v>
       </c>
-      <c r="C14" t="s">
-        <v>29</v>
+      <c r="C14" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -4108,8 +4108,8 @@
       <c r="B15" t="s">
         <v>337</v>
       </c>
-      <c r="C15" t="s">
-        <v>29</v>
+      <c r="C15" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -4119,8 +4119,8 @@
       <c r="B16" t="s">
         <v>339</v>
       </c>
-      <c r="C16" t="s">
-        <v>29</v>
+      <c r="C16" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -4130,8 +4130,8 @@
       <c r="B17" t="s">
         <v>341</v>
       </c>
-      <c r="C17" t="s">
-        <v>29</v>
+      <c r="C17" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -4141,8 +4141,8 @@
       <c r="B18" t="s">
         <v>343</v>
       </c>
-      <c r="C18" t="s">
-        <v>29</v>
+      <c r="C18" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -4152,8 +4152,8 @@
       <c r="B19" t="s">
         <v>345</v>
       </c>
-      <c r="C19" t="s">
-        <v>29</v>
+      <c r="C19" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -4163,8 +4163,8 @@
       <c r="B20" t="s">
         <v>68</v>
       </c>
-      <c r="C20" t="s">
-        <v>29</v>
+      <c r="C20" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -4174,8 +4174,8 @@
       <c r="B21" t="s">
         <v>347</v>
       </c>
-      <c r="C21" t="s">
-        <v>29</v>
+      <c r="C21" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -4185,8 +4185,8 @@
       <c r="B22" t="s">
         <v>68</v>
       </c>
-      <c r="C22" t="s">
-        <v>29</v>
+      <c r="C22" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -4196,8 +4196,8 @@
       <c r="B23" t="s">
         <v>350</v>
       </c>
-      <c r="C23" t="s">
-        <v>29</v>
+      <c r="C23" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -4207,8 +4207,8 @@
       <c r="B24" t="s">
         <v>352</v>
       </c>
-      <c r="C24" t="s">
-        <v>29</v>
+      <c r="C24" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -4218,8 +4218,8 @@
       <c r="B25" t="s">
         <v>354</v>
       </c>
-      <c r="C25" t="s">
-        <v>29</v>
+      <c r="C25" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -4229,8 +4229,8 @@
       <c r="B26" t="s">
         <v>356</v>
       </c>
-      <c r="C26" t="s">
-        <v>29</v>
+      <c r="C26" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -17716,8 +17716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AO78"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17772,7 +17772,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>22</v>
@@ -17789,7 +17789,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>53</v>
@@ -17806,7 +17806,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>22</v>
@@ -17865,7 +17865,7 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
         <v>41</v>
@@ -17885,7 +17885,7 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
         <v>42</v>
@@ -17905,7 +17905,7 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B13" t="s">
         <v>43</v>
@@ -17925,7 +17925,7 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
         <v>44</v>
@@ -17945,7 +17945,7 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B15" t="s">
         <v>48</v>
@@ -18190,7 +18190,7 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B32" t="s">
         <v>16</v>
@@ -18347,7 +18347,7 @@
     </row>
     <row r="44" spans="1:25">
       <c r="A44" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B44" t="s">
         <v>16</v>
@@ -18361,7 +18361,7 @@
     </row>
     <row r="45" spans="1:25">
       <c r="A45" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B45" t="s">
         <v>16</v>
@@ -19646,7 +19646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:XFB45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+    <sheetView topLeftCell="A26" workbookViewId="0">
       <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Excel and OR files updated
</commit_message>
<xml_diff>
--- a/src/com/supplierconnection/xls/TestSuite1.xlsx
+++ b/src/com/supplierconnection/xls/TestSuite1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12315" windowHeight="2055"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12315" windowHeight="2055" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4890" uniqueCount="1110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4892" uniqueCount="1110">
   <si>
     <t>TCID</t>
   </si>
@@ -2607,9 +2607,6 @@
     <t>sc_adddone</t>
   </si>
   <si>
-    <t>SC_removeadminaccess</t>
-  </si>
-  <si>
     <t>sc_removingaccesswindow</t>
   </si>
   <si>
@@ -3367,6 +3364,9 @@
   </si>
   <si>
     <t>teston.bluemix@gmail.com</t>
+  </si>
+  <si>
+    <t>SC_removeadminaccess2</t>
   </si>
 </sst>
 </file>
@@ -3938,8 +3938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4202,7 +4202,7 @@
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="28" t="s">
         <v>345</v>
       </c>
       <c r="B24" t="s">
@@ -4213,7 +4213,7 @@
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="28" t="s">
         <v>347</v>
       </c>
       <c r="B25" t="s">
@@ -4224,7 +4224,7 @@
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="24" t="s">
+      <c r="A26" s="18" t="s">
         <v>349</v>
       </c>
       <c r="B26" t="s">
@@ -4236,10 +4236,10 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="B27" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="C27" s="54" t="s">
         <v>4</v>
@@ -4252,10 +4252,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G1109"/>
+  <dimension ref="A1:G1110"/>
   <sheetViews>
-    <sheetView topLeftCell="A509" workbookViewId="0">
-      <selection activeCell="A523" sqref="A523"/>
+    <sheetView tabSelected="1" topLeftCell="A999" workbookViewId="0">
+      <selection activeCell="B1013" sqref="B1013"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5507,7 +5507,7 @@
       </c>
       <c r="C93" s="21"/>
       <c r="D93" s="21" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="E93" s="30" t="s">
         <v>4</v>
@@ -5522,7 +5522,7 @@
       </c>
       <c r="C94" s="21"/>
       <c r="D94" s="21" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="E94" s="21" t="s">
         <v>4</v>
@@ -5537,7 +5537,7 @@
       </c>
       <c r="C95" s="21"/>
       <c r="D95" s="21" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="E95" s="21" t="s">
         <v>4</v>
@@ -5552,7 +5552,7 @@
       </c>
       <c r="C96" s="21"/>
       <c r="D96" s="21" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="E96" s="21" t="s">
         <v>4</v>
@@ -17923,7 +17923,7 @@
       <c r="E1000" s="30"/>
     </row>
     <row r="1001" spans="1:5">
-      <c r="A1001" s="51" t="s">
+      <c r="A1001" s="31" t="s">
         <v>343</v>
       </c>
       <c r="B1001" s="31" t="s">
@@ -17988,11 +17988,9 @@
         <v>343</v>
       </c>
       <c r="B1006" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1006" s="31" t="s">
-        <v>856</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C1006" s="31"/>
       <c r="D1006" s="31"/>
       <c r="E1006" s="30"/>
     </row>
@@ -18001,14 +17999,12 @@
         <v>343</v>
       </c>
       <c r="B1007" s="31" t="s">
-        <v>226</v>
+        <v>8</v>
       </c>
       <c r="C1007" s="31" t="s">
-        <v>857</v>
-      </c>
-      <c r="D1007" s="31" t="s">
-        <v>857</v>
-      </c>
+        <v>1109</v>
+      </c>
+      <c r="D1007" s="31"/>
       <c r="E1007" s="30"/>
     </row>
     <row r="1008" spans="1:5">
@@ -18016,12 +18012,14 @@
         <v>343</v>
       </c>
       <c r="B1008" s="31" t="s">
-        <v>8</v>
+        <v>226</v>
       </c>
       <c r="C1008" s="31" t="s">
-        <v>858</v>
-      </c>
-      <c r="D1008" s="31"/>
+        <v>856</v>
+      </c>
+      <c r="D1008" s="31" t="s">
+        <v>856</v>
+      </c>
       <c r="E1008" s="30"/>
     </row>
     <row r="1009" spans="1:5">
@@ -18029,14 +18027,12 @@
         <v>343</v>
       </c>
       <c r="B1009" s="31" t="s">
-        <v>226</v>
+        <v>8</v>
       </c>
       <c r="C1009" s="31" t="s">
-        <v>859</v>
-      </c>
-      <c r="D1009" s="31" t="s">
-        <v>859</v>
-      </c>
+        <v>857</v>
+      </c>
+      <c r="D1009" s="31"/>
       <c r="E1009" s="30"/>
     </row>
     <row r="1010" spans="1:5">
@@ -18044,12 +18040,14 @@
         <v>343</v>
       </c>
       <c r="B1010" s="31" t="s">
-        <v>8</v>
+        <v>226</v>
       </c>
       <c r="C1010" s="31" t="s">
-        <v>860</v>
-      </c>
-      <c r="D1010" s="31"/>
+        <v>858</v>
+      </c>
+      <c r="D1010" s="31" t="s">
+        <v>858</v>
+      </c>
       <c r="E1010" s="30"/>
     </row>
     <row r="1011" spans="1:5">
@@ -18057,22 +18055,22 @@
         <v>343</v>
       </c>
       <c r="B1011" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1011" s="31"/>
+        <v>8</v>
+      </c>
+      <c r="C1011" s="31" t="s">
+        <v>859</v>
+      </c>
       <c r="D1011" s="31"/>
       <c r="E1011" s="30"/>
     </row>
     <row r="1012" spans="1:5">
-      <c r="A1012" s="51" t="s">
+      <c r="A1012" s="31" t="s">
         <v>343</v>
       </c>
       <c r="B1012" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1012" s="52" t="s">
-        <v>861</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C1012" s="31"/>
       <c r="D1012" s="31"/>
       <c r="E1012" s="30"/>
     </row>
@@ -18081,14 +18079,12 @@
         <v>343</v>
       </c>
       <c r="B1013" s="31" t="s">
-        <v>226</v>
-      </c>
-      <c r="C1013" s="31" t="s">
-        <v>862</v>
-      </c>
-      <c r="D1013" s="31" t="s">
-        <v>862</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C1013" s="52" t="s">
+        <v>860</v>
+      </c>
+      <c r="D1013" s="31"/>
       <c r="E1013" s="30"/>
     </row>
     <row r="1014" spans="1:5">
@@ -18098,11 +18094,11 @@
       <c r="B1014" s="31" t="s">
         <v>226</v>
       </c>
-      <c r="C1014" s="51" t="s">
-        <v>857</v>
+      <c r="C1014" s="31" t="s">
+        <v>861</v>
       </c>
       <c r="D1014" s="31" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="E1014" s="30"/>
     </row>
@@ -18111,63 +18107,65 @@
         <v>343</v>
       </c>
       <c r="B1015" s="31" t="s">
-        <v>8</v>
+        <v>226</v>
       </c>
       <c r="C1015" s="51" t="s">
-        <v>858</v>
-      </c>
-      <c r="D1015" s="31"/>
+        <v>856</v>
+      </c>
+      <c r="D1015" s="31" t="s">
+        <v>862</v>
+      </c>
       <c r="E1015" s="30"/>
     </row>
     <row r="1016" spans="1:5">
-      <c r="A1016" s="31" t="s">
+      <c r="A1016" s="51" t="s">
         <v>343</v>
       </c>
       <c r="B1016" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1016" s="51" t="s">
+        <v>857</v>
+      </c>
+      <c r="D1016" s="31"/>
+      <c r="E1016" s="30"/>
+    </row>
+    <row r="1017" spans="1:5">
+      <c r="A1017" s="31" t="s">
+        <v>343</v>
+      </c>
+      <c r="B1017" s="31" t="s">
         <v>226</v>
       </c>
-      <c r="C1016" s="31" t="s">
+      <c r="C1017" s="31" t="s">
+        <v>863</v>
+      </c>
+      <c r="D1017" s="31" t="s">
         <v>864</v>
       </c>
-      <c r="D1016" s="31" t="s">
-        <v>865</v>
-      </c>
-      <c r="E1016" s="30"/>
-    </row>
-    <row r="1017" spans="1:5">
-      <c r="A1017" s="51" t="s">
+      <c r="E1017" s="30"/>
+    </row>
+    <row r="1018" spans="1:5">
+      <c r="A1018" s="51" t="s">
         <v>343</v>
       </c>
-      <c r="B1017" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1017" s="31" t="s">
-        <v>860</v>
-      </c>
-      <c r="D1017" s="31"/>
-      <c r="E1017" s="30"/>
-    </row>
-    <row r="1018" spans="1:5">
-      <c r="A1018" s="31" t="s">
-        <v>343</v>
-      </c>
       <c r="B1018" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1018" s="31"/>
+        <v>8</v>
+      </c>
+      <c r="C1018" s="31" t="s">
+        <v>859</v>
+      </c>
       <c r="D1018" s="31"/>
       <c r="E1018" s="30"/>
     </row>
     <row r="1019" spans="1:5">
-      <c r="A1019" s="51" t="s">
+      <c r="A1019" s="31" t="s">
         <v>343</v>
       </c>
       <c r="B1019" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1019" s="31" t="s">
-        <v>866</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C1019" s="31"/>
       <c r="D1019" s="31"/>
       <c r="E1019" s="30"/>
     </row>
@@ -18179,22 +18177,22 @@
         <v>8</v>
       </c>
       <c r="C1020" s="31" t="s">
-        <v>858</v>
+        <v>865</v>
       </c>
       <c r="D1020" s="31"/>
       <c r="E1020" s="30"/>
     </row>
     <row r="1021" spans="1:5">
-      <c r="A1021" s="53" t="s">
-        <v>345</v>
+      <c r="A1021" s="51" t="s">
+        <v>343</v>
       </c>
       <c r="B1021" s="31" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1021" s="31"/>
-      <c r="D1021" s="31" t="s">
-        <v>15</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C1021" s="31" t="s">
+        <v>857</v>
+      </c>
+      <c r="D1021" s="31"/>
       <c r="E1021" s="30"/>
     </row>
     <row r="1022" spans="1:5">
@@ -18202,12 +18200,12 @@
         <v>345</v>
       </c>
       <c r="B1022" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1022" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1022" s="31"/>
+        <v>6</v>
+      </c>
+      <c r="C1022" s="31"/>
+      <c r="D1022" s="31" t="s">
+        <v>15</v>
+      </c>
       <c r="E1022" s="30"/>
     </row>
     <row r="1023" spans="1:5">
@@ -18215,36 +18213,36 @@
         <v>345</v>
       </c>
       <c r="B1023" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1023" s="31"/>
-      <c r="D1023" s="31" t="s">
-        <v>40</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C1023" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1023" s="31"/>
       <c r="E1023" s="30"/>
     </row>
     <row r="1024" spans="1:5">
       <c r="A1024" s="53" t="s">
         <v>345</v>
       </c>
-      <c r="B1024" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1024" s="30" t="s">
-        <v>833</v>
-      </c>
-      <c r="D1024" s="30"/>
+      <c r="B1024" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1024" s="31"/>
+      <c r="D1024" s="31" t="s">
+        <v>40</v>
+      </c>
       <c r="E1024" s="30"/>
     </row>
     <row r="1025" spans="1:5">
       <c r="A1025" s="53" t="s">
         <v>345</v>
       </c>
-      <c r="B1025" s="31" t="s">
-        <v>475</v>
+      <c r="B1025" s="30" t="s">
+        <v>8</v>
       </c>
       <c r="C1025" s="30" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="D1025" s="30"/>
       <c r="E1025" s="30"/>
@@ -18253,11 +18251,11 @@
       <c r="A1026" s="53" t="s">
         <v>345</v>
       </c>
-      <c r="B1026" s="30" t="s">
-        <v>8</v>
+      <c r="B1026" s="31" t="s">
+        <v>475</v>
       </c>
       <c r="C1026" s="30" t="s">
-        <v>867</v>
+        <v>834</v>
       </c>
       <c r="D1026" s="30"/>
       <c r="E1026" s="30"/>
@@ -18266,10 +18264,12 @@
       <c r="A1027" s="53" t="s">
         <v>345</v>
       </c>
-      <c r="B1027" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1027" s="30"/>
+      <c r="B1027" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1027" s="30" t="s">
+        <v>866</v>
+      </c>
       <c r="D1027" s="30"/>
       <c r="E1027" s="30"/>
     </row>
@@ -18277,15 +18277,11 @@
       <c r="A1028" s="53" t="s">
         <v>345</v>
       </c>
-      <c r="B1028" s="30" t="s">
-        <v>226</v>
-      </c>
-      <c r="C1028" s="30" t="s">
-        <v>868</v>
-      </c>
-      <c r="D1028" s="30" t="s">
-        <v>868</v>
-      </c>
+      <c r="B1028" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1028" s="30"/>
+      <c r="D1028" s="30"/>
       <c r="E1028" s="30"/>
     </row>
     <row r="1029" spans="1:5">
@@ -18293,12 +18289,14 @@
         <v>345</v>
       </c>
       <c r="B1029" s="30" t="s">
-        <v>8</v>
+        <v>226</v>
       </c>
       <c r="C1029" s="30" t="s">
-        <v>869</v>
-      </c>
-      <c r="D1029" s="30"/>
+        <v>867</v>
+      </c>
+      <c r="D1029" s="30" t="s">
+        <v>867</v>
+      </c>
       <c r="E1029" s="30"/>
     </row>
     <row r="1030" spans="1:5">
@@ -18306,28 +18304,26 @@
         <v>345</v>
       </c>
       <c r="B1030" s="30" t="s">
-        <v>226</v>
+        <v>8</v>
       </c>
       <c r="C1030" s="30" t="s">
-        <v>839</v>
-      </c>
-      <c r="D1030" s="30" t="s">
-        <v>839</v>
-      </c>
+        <v>868</v>
+      </c>
+      <c r="D1030" s="30"/>
       <c r="E1030" s="30"/>
     </row>
     <row r="1031" spans="1:5">
       <c r="A1031" s="53" t="s">
         <v>345</v>
       </c>
-      <c r="B1031" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1031" s="31" t="s">
-        <v>840</v>
+      <c r="B1031" s="30" t="s">
+        <v>226</v>
+      </c>
+      <c r="C1031" s="30" t="s">
+        <v>839</v>
       </c>
       <c r="D1031" s="30" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="E1031" s="30"/>
     </row>
@@ -18335,13 +18331,15 @@
       <c r="A1032" s="53" t="s">
         <v>345</v>
       </c>
-      <c r="B1032" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1032" s="30" t="s">
-        <v>869</v>
-      </c>
-      <c r="D1032" s="30"/>
+      <c r="B1032" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1032" s="31" t="s">
+        <v>840</v>
+      </c>
+      <c r="D1032" s="30" t="s">
+        <v>841</v>
+      </c>
       <c r="E1032" s="30"/>
     </row>
     <row r="1033" spans="1:5">
@@ -18349,28 +18347,26 @@
         <v>345</v>
       </c>
       <c r="B1033" s="30" t="s">
-        <v>226</v>
+        <v>8</v>
       </c>
       <c r="C1033" s="30" t="s">
-        <v>839</v>
-      </c>
-      <c r="D1033" s="30" t="s">
-        <v>839</v>
-      </c>
+        <v>868</v>
+      </c>
+      <c r="D1033" s="30"/>
       <c r="E1033" s="30"/>
     </row>
     <row r="1034" spans="1:5">
       <c r="A1034" s="53" t="s">
         <v>345</v>
       </c>
-      <c r="B1034" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1034" s="31" t="s">
-        <v>840</v>
-      </c>
-      <c r="D1034" s="31" t="s">
-        <v>842</v>
+      <c r="B1034" s="30" t="s">
+        <v>226</v>
+      </c>
+      <c r="C1034" s="30" t="s">
+        <v>839</v>
+      </c>
+      <c r="D1034" s="30" t="s">
+        <v>839</v>
       </c>
       <c r="E1034" s="30"/>
     </row>
@@ -18379,10 +18375,14 @@
         <v>345</v>
       </c>
       <c r="B1035" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1035" s="31"/>
-      <c r="D1035" s="31"/>
+        <v>9</v>
+      </c>
+      <c r="C1035" s="31" t="s">
+        <v>840</v>
+      </c>
+      <c r="D1035" s="31" t="s">
+        <v>842</v>
+      </c>
       <c r="E1035" s="30"/>
     </row>
     <row r="1036" spans="1:5">
@@ -18390,12 +18390,10 @@
         <v>345</v>
       </c>
       <c r="B1036" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1036" s="31" t="s">
-        <v>869</v>
-      </c>
-      <c r="D1036" s="30"/>
+        <v>51</v>
+      </c>
+      <c r="C1036" s="31"/>
+      <c r="D1036" s="31"/>
       <c r="E1036" s="30"/>
     </row>
     <row r="1037" spans="1:5">
@@ -18403,9 +18401,11 @@
         <v>345</v>
       </c>
       <c r="B1037" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1037" s="31"/>
+        <v>8</v>
+      </c>
+      <c r="C1037" s="31" t="s">
+        <v>868</v>
+      </c>
       <c r="D1037" s="30"/>
       <c r="E1037" s="30"/>
     </row>
@@ -18414,11 +18414,9 @@
         <v>345</v>
       </c>
       <c r="B1038" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1038" s="31" t="s">
-        <v>870</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C1038" s="31"/>
       <c r="D1038" s="30"/>
       <c r="E1038" s="30"/>
     </row>
@@ -18427,9 +18425,11 @@
         <v>345</v>
       </c>
       <c r="B1039" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1039" s="31"/>
+        <v>8</v>
+      </c>
+      <c r="C1039" s="31" t="s">
+        <v>869</v>
+      </c>
       <c r="D1039" s="30"/>
       <c r="E1039" s="30"/>
     </row>
@@ -18437,29 +18437,25 @@
       <c r="A1040" s="53" t="s">
         <v>345</v>
       </c>
-      <c r="B1040" s="30" t="s">
-        <v>226</v>
-      </c>
-      <c r="C1040" s="31" t="s">
-        <v>844</v>
-      </c>
-      <c r="D1040" s="30" t="s">
-        <v>844</v>
-      </c>
+      <c r="B1040" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1040" s="31"/>
+      <c r="D1040" s="30"/>
       <c r="E1040" s="30"/>
     </row>
     <row r="1041" spans="1:5">
       <c r="A1041" s="53" t="s">
         <v>345</v>
       </c>
-      <c r="B1041" s="31" t="s">
-        <v>9</v>
+      <c r="B1041" s="30" t="s">
+        <v>226</v>
       </c>
       <c r="C1041" s="31" t="s">
-        <v>840</v>
+        <v>844</v>
       </c>
       <c r="D1041" s="30" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="E1041" s="30"/>
     </row>
@@ -18468,10 +18464,14 @@
         <v>345</v>
       </c>
       <c r="B1042" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1042" s="31"/>
-      <c r="D1042" s="31"/>
+        <v>9</v>
+      </c>
+      <c r="C1042" s="31" t="s">
+        <v>840</v>
+      </c>
+      <c r="D1042" s="30" t="s">
+        <v>845</v>
+      </c>
       <c r="E1042" s="30"/>
     </row>
     <row r="1043" spans="1:5">
@@ -18479,12 +18479,10 @@
         <v>345</v>
       </c>
       <c r="B1043" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1043" s="30" t="s">
-        <v>869</v>
-      </c>
-      <c r="D1043" s="30"/>
+        <v>51</v>
+      </c>
+      <c r="C1043" s="31"/>
+      <c r="D1043" s="31"/>
       <c r="E1043" s="30"/>
     </row>
     <row r="1044" spans="1:5">
@@ -18492,9 +18490,11 @@
         <v>345</v>
       </c>
       <c r="B1044" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1044" s="31"/>
+        <v>8</v>
+      </c>
+      <c r="C1044" s="30" t="s">
+        <v>868</v>
+      </c>
       <c r="D1044" s="30"/>
       <c r="E1044" s="30"/>
     </row>
@@ -18503,11 +18503,9 @@
         <v>345</v>
       </c>
       <c r="B1045" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1045" s="31" t="s">
-        <v>843</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C1045" s="31"/>
       <c r="D1045" s="30"/>
       <c r="E1045" s="30"/>
     </row>
@@ -18515,29 +18513,27 @@
       <c r="A1046" s="53" t="s">
         <v>345</v>
       </c>
-      <c r="B1046" s="30" t="s">
-        <v>226</v>
+      <c r="B1046" s="31" t="s">
+        <v>8</v>
       </c>
       <c r="C1046" s="31" t="s">
-        <v>846</v>
-      </c>
-      <c r="D1046" s="30" t="s">
-        <v>846</v>
-      </c>
+        <v>843</v>
+      </c>
+      <c r="D1046" s="30"/>
       <c r="E1046" s="30"/>
     </row>
     <row r="1047" spans="1:5">
       <c r="A1047" s="53" t="s">
         <v>345</v>
       </c>
-      <c r="B1047" s="31" t="s">
-        <v>9</v>
+      <c r="B1047" s="30" t="s">
+        <v>226</v>
       </c>
       <c r="C1047" s="31" t="s">
-        <v>840</v>
+        <v>846</v>
       </c>
       <c r="D1047" s="30" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="E1047" s="30"/>
     </row>
@@ -18546,10 +18542,14 @@
         <v>345</v>
       </c>
       <c r="B1048" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1048" s="31"/>
-      <c r="D1048" s="31"/>
+        <v>9</v>
+      </c>
+      <c r="C1048" s="31" t="s">
+        <v>840</v>
+      </c>
+      <c r="D1048" s="30" t="s">
+        <v>847</v>
+      </c>
       <c r="E1048" s="30"/>
     </row>
     <row r="1049" spans="1:5">
@@ -18557,12 +18557,10 @@
         <v>345</v>
       </c>
       <c r="B1049" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1049" s="30" t="s">
-        <v>869</v>
-      </c>
-      <c r="D1049" s="30"/>
+        <v>51</v>
+      </c>
+      <c r="C1049" s="31"/>
+      <c r="D1049" s="31"/>
       <c r="E1049" s="30"/>
     </row>
     <row r="1050" spans="1:5">
@@ -18570,9 +18568,11 @@
         <v>345</v>
       </c>
       <c r="B1050" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1050" s="31"/>
+        <v>8</v>
+      </c>
+      <c r="C1050" s="30" t="s">
+        <v>868</v>
+      </c>
       <c r="D1050" s="30"/>
       <c r="E1050" s="30"/>
     </row>
@@ -18581,11 +18581,9 @@
         <v>345</v>
       </c>
       <c r="B1051" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1051" s="31" t="s">
-        <v>843</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C1051" s="31"/>
       <c r="D1051" s="30"/>
       <c r="E1051" s="30"/>
     </row>
@@ -18593,29 +18591,27 @@
       <c r="A1052" s="53" t="s">
         <v>345</v>
       </c>
-      <c r="B1052" s="30" t="s">
-        <v>226</v>
+      <c r="B1052" s="31" t="s">
+        <v>8</v>
       </c>
       <c r="C1052" s="31" t="s">
-        <v>848</v>
-      </c>
-      <c r="D1052" s="30" t="s">
-        <v>848</v>
-      </c>
+        <v>843</v>
+      </c>
+      <c r="D1052" s="30"/>
       <c r="E1052" s="30"/>
     </row>
     <row r="1053" spans="1:5">
       <c r="A1053" s="53" t="s">
         <v>345</v>
       </c>
-      <c r="B1053" s="31" t="s">
-        <v>9</v>
+      <c r="B1053" s="30" t="s">
+        <v>226</v>
       </c>
       <c r="C1053" s="31" t="s">
-        <v>840</v>
+        <v>848</v>
       </c>
       <c r="D1053" s="30" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="E1053" s="30"/>
     </row>
@@ -18624,10 +18620,14 @@
         <v>345</v>
       </c>
       <c r="B1054" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1054" s="31"/>
-      <c r="D1054" s="31"/>
+        <v>9</v>
+      </c>
+      <c r="C1054" s="31" t="s">
+        <v>840</v>
+      </c>
+      <c r="D1054" s="30" t="s">
+        <v>849</v>
+      </c>
       <c r="E1054" s="30"/>
     </row>
     <row r="1055" spans="1:5">
@@ -18635,12 +18635,10 @@
         <v>345</v>
       </c>
       <c r="B1055" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1055" s="30" t="s">
-        <v>869</v>
-      </c>
-      <c r="D1055" s="30"/>
+        <v>51</v>
+      </c>
+      <c r="C1055" s="31"/>
+      <c r="D1055" s="31"/>
       <c r="E1055" s="30"/>
     </row>
     <row r="1056" spans="1:5">
@@ -18648,9 +18646,11 @@
         <v>345</v>
       </c>
       <c r="B1056" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1056" s="31"/>
+        <v>8</v>
+      </c>
+      <c r="C1056" s="30" t="s">
+        <v>868</v>
+      </c>
       <c r="D1056" s="30"/>
       <c r="E1056" s="30"/>
     </row>
@@ -18659,11 +18659,9 @@
         <v>345</v>
       </c>
       <c r="B1057" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1057" s="31" t="s">
-        <v>843</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C1057" s="31"/>
       <c r="D1057" s="30"/>
       <c r="E1057" s="30"/>
     </row>
@@ -18671,29 +18669,27 @@
       <c r="A1058" s="53" t="s">
         <v>345</v>
       </c>
-      <c r="B1058" s="30" t="s">
-        <v>226</v>
+      <c r="B1058" s="31" t="s">
+        <v>8</v>
       </c>
       <c r="C1058" s="31" t="s">
-        <v>850</v>
-      </c>
-      <c r="D1058" s="31" t="s">
-        <v>850</v>
-      </c>
+        <v>843</v>
+      </c>
+      <c r="D1058" s="30"/>
       <c r="E1058" s="30"/>
     </row>
     <row r="1059" spans="1:5">
       <c r="A1059" s="53" t="s">
         <v>345</v>
       </c>
-      <c r="B1059" s="31" t="s">
-        <v>9</v>
+      <c r="B1059" s="30" t="s">
+        <v>226</v>
       </c>
       <c r="C1059" s="31" t="s">
-        <v>840</v>
-      </c>
-      <c r="D1059" s="30" t="s">
-        <v>851</v>
+        <v>850</v>
+      </c>
+      <c r="D1059" s="31" t="s">
+        <v>850</v>
       </c>
       <c r="E1059" s="30"/>
     </row>
@@ -18702,10 +18698,14 @@
         <v>345</v>
       </c>
       <c r="B1060" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1060" s="31"/>
-      <c r="D1060" s="31"/>
+        <v>9</v>
+      </c>
+      <c r="C1060" s="31" t="s">
+        <v>840</v>
+      </c>
+      <c r="D1060" s="30" t="s">
+        <v>851</v>
+      </c>
       <c r="E1060" s="30"/>
     </row>
     <row r="1061" spans="1:5">
@@ -18713,12 +18713,10 @@
         <v>345</v>
       </c>
       <c r="B1061" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1061" s="30" t="s">
-        <v>869</v>
-      </c>
-      <c r="D1061" s="30"/>
+        <v>51</v>
+      </c>
+      <c r="C1061" s="31"/>
+      <c r="D1061" s="31"/>
       <c r="E1061" s="30"/>
     </row>
     <row r="1062" spans="1:5">
@@ -18726,9 +18724,11 @@
         <v>345</v>
       </c>
       <c r="B1062" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1062" s="31"/>
+        <v>8</v>
+      </c>
+      <c r="C1062" s="30" t="s">
+        <v>868</v>
+      </c>
       <c r="D1062" s="30"/>
       <c r="E1062" s="30"/>
     </row>
@@ -18737,11 +18737,9 @@
         <v>345</v>
       </c>
       <c r="B1063" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1063" s="31" t="s">
-        <v>843</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C1063" s="31"/>
       <c r="D1063" s="30"/>
       <c r="E1063" s="30"/>
     </row>
@@ -18749,29 +18747,27 @@
       <c r="A1064" s="53" t="s">
         <v>345</v>
       </c>
-      <c r="B1064" s="30" t="s">
-        <v>226</v>
+      <c r="B1064" s="31" t="s">
+        <v>8</v>
       </c>
       <c r="C1064" s="31" t="s">
-        <v>852</v>
-      </c>
-      <c r="D1064" s="31" t="s">
-        <v>852</v>
-      </c>
+        <v>843</v>
+      </c>
+      <c r="D1064" s="30"/>
       <c r="E1064" s="30"/>
     </row>
     <row r="1065" spans="1:5">
       <c r="A1065" s="53" t="s">
         <v>345</v>
       </c>
-      <c r="B1065" s="31" t="s">
-        <v>9</v>
+      <c r="B1065" s="30" t="s">
+        <v>226</v>
       </c>
       <c r="C1065" s="31" t="s">
-        <v>840</v>
-      </c>
-      <c r="D1065" s="30" t="s">
-        <v>853</v>
+        <v>852</v>
+      </c>
+      <c r="D1065" s="31" t="s">
+        <v>852</v>
       </c>
       <c r="E1065" s="30"/>
     </row>
@@ -18780,10 +18776,14 @@
         <v>345</v>
       </c>
       <c r="B1066" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1066" s="31"/>
-      <c r="D1066" s="31"/>
+        <v>9</v>
+      </c>
+      <c r="C1066" s="31" t="s">
+        <v>840</v>
+      </c>
+      <c r="D1066" s="30" t="s">
+        <v>853</v>
+      </c>
       <c r="E1066" s="30"/>
     </row>
     <row r="1067" spans="1:5">
@@ -18791,12 +18791,10 @@
         <v>345</v>
       </c>
       <c r="B1067" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1067" s="30" t="s">
-        <v>869</v>
-      </c>
-      <c r="D1067" s="30"/>
+        <v>51</v>
+      </c>
+      <c r="C1067" s="31"/>
+      <c r="D1067" s="31"/>
       <c r="E1067" s="30"/>
     </row>
     <row r="1068" spans="1:5">
@@ -18804,9 +18802,11 @@
         <v>345</v>
       </c>
       <c r="B1068" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1068" s="31"/>
+        <v>8</v>
+      </c>
+      <c r="C1068" s="30" t="s">
+        <v>868</v>
+      </c>
       <c r="D1068" s="30"/>
       <c r="E1068" s="30"/>
     </row>
@@ -18814,29 +18814,25 @@
       <c r="A1069" s="53" t="s">
         <v>345</v>
       </c>
-      <c r="B1069" s="30" t="s">
-        <v>226</v>
-      </c>
-      <c r="C1069" s="31" t="s">
-        <v>854</v>
-      </c>
-      <c r="D1069" s="31" t="s">
-        <v>854</v>
-      </c>
+      <c r="B1069" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1069" s="31"/>
+      <c r="D1069" s="30"/>
       <c r="E1069" s="30"/>
     </row>
     <row r="1070" spans="1:5">
       <c r="A1070" s="53" t="s">
         <v>345</v>
       </c>
-      <c r="B1070" s="31" t="s">
-        <v>9</v>
+      <c r="B1070" s="30" t="s">
+        <v>226</v>
       </c>
       <c r="C1070" s="31" t="s">
-        <v>840</v>
+        <v>854</v>
       </c>
       <c r="D1070" s="31" t="s">
-        <v>840</v>
+        <v>854</v>
       </c>
       <c r="E1070" s="30"/>
     </row>
@@ -18845,10 +18841,14 @@
         <v>345</v>
       </c>
       <c r="B1071" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1071" s="31"/>
-      <c r="D1071" s="31"/>
+        <v>9</v>
+      </c>
+      <c r="C1071" s="31" t="s">
+        <v>840</v>
+      </c>
+      <c r="D1071" s="31" t="s">
+        <v>840</v>
+      </c>
       <c r="E1071" s="30"/>
     </row>
     <row r="1072" spans="1:5">
@@ -18856,11 +18856,9 @@
         <v>345</v>
       </c>
       <c r="B1072" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1072" s="30" t="s">
-        <v>869</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C1072" s="31"/>
       <c r="D1072" s="31"/>
       <c r="E1072" s="30"/>
     </row>
@@ -18869,9 +18867,11 @@
         <v>345</v>
       </c>
       <c r="B1073" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1073" s="31"/>
+        <v>8</v>
+      </c>
+      <c r="C1073" s="30" t="s">
+        <v>868</v>
+      </c>
       <c r="D1073" s="31"/>
       <c r="E1073" s="30"/>
     </row>
@@ -18880,11 +18880,9 @@
         <v>345</v>
       </c>
       <c r="B1074" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1074" s="31" t="s">
-        <v>843</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C1074" s="31"/>
       <c r="D1074" s="31"/>
       <c r="E1074" s="30"/>
     </row>
@@ -18896,7 +18894,7 @@
         <v>8</v>
       </c>
       <c r="C1075" s="31" t="s">
-        <v>855</v>
+        <v>843</v>
       </c>
       <c r="D1075" s="31"/>
       <c r="E1075" s="30"/>
@@ -18908,10 +18906,10 @@
       <c r="B1076" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C1076" s="30" t="s">
-        <v>871</v>
-      </c>
-      <c r="D1076" s="30"/>
+      <c r="C1076" s="31" t="s">
+        <v>855</v>
+      </c>
+      <c r="D1076" s="31"/>
       <c r="E1076" s="30"/>
     </row>
     <row r="1077" spans="1:5">
@@ -18922,22 +18920,22 @@
         <v>8</v>
       </c>
       <c r="C1077" s="30" t="s">
-        <v>858</v>
+        <v>870</v>
       </c>
       <c r="D1077" s="30"/>
       <c r="E1077" s="30"/>
     </row>
     <row r="1078" spans="1:5">
       <c r="A1078" s="53" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B1078" s="31" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1078" s="31"/>
-      <c r="D1078" s="31" t="s">
-        <v>15</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C1078" s="30" t="s">
+        <v>857</v>
+      </c>
+      <c r="D1078" s="30"/>
       <c r="E1078" s="30"/>
     </row>
     <row r="1079" spans="1:5">
@@ -18945,12 +18943,12 @@
         <v>347</v>
       </c>
       <c r="B1079" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1079" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1079" s="31"/>
+        <v>6</v>
+      </c>
+      <c r="C1079" s="31"/>
+      <c r="D1079" s="31" t="s">
+        <v>15</v>
+      </c>
       <c r="E1079" s="30"/>
     </row>
     <row r="1080" spans="1:5">
@@ -18958,36 +18956,36 @@
         <v>347</v>
       </c>
       <c r="B1080" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1080" s="31"/>
-      <c r="D1080" s="31" t="s">
-        <v>40</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C1080" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1080" s="31"/>
       <c r="E1080" s="30"/>
     </row>
     <row r="1081" spans="1:5">
       <c r="A1081" s="53" t="s">
         <v>347</v>
       </c>
-      <c r="B1081" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1081" s="30" t="s">
-        <v>833</v>
-      </c>
-      <c r="D1081" s="30"/>
+      <c r="B1081" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1081" s="31"/>
+      <c r="D1081" s="31" t="s">
+        <v>40</v>
+      </c>
       <c r="E1081" s="30"/>
     </row>
     <row r="1082" spans="1:5">
       <c r="A1082" s="53" t="s">
         <v>347</v>
       </c>
-      <c r="B1082" s="31" t="s">
-        <v>475</v>
+      <c r="B1082" s="30" t="s">
+        <v>8</v>
       </c>
       <c r="C1082" s="30" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="D1082" s="30"/>
       <c r="E1082" s="30"/>
@@ -18996,39 +18994,37 @@
       <c r="A1083" s="53" t="s">
         <v>347</v>
       </c>
-      <c r="B1083" s="30" t="s">
-        <v>8</v>
+      <c r="B1083" s="31" t="s">
+        <v>475</v>
       </c>
       <c r="C1083" s="30" t="s">
-        <v>836</v>
-      </c>
-      <c r="D1083" s="31"/>
+        <v>834</v>
+      </c>
+      <c r="D1083" s="30"/>
       <c r="E1083" s="30"/>
     </row>
     <row r="1084" spans="1:5">
       <c r="A1084" s="53" t="s">
         <v>347</v>
       </c>
-      <c r="B1084" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1084" s="30"/>
+      <c r="B1084" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1084" s="30" t="s">
+        <v>836</v>
+      </c>
       <c r="D1084" s="31"/>
       <c r="E1084" s="30"/>
     </row>
     <row r="1085" spans="1:5">
-      <c r="A1085" s="31" t="s">
+      <c r="A1085" s="53" t="s">
         <v>347</v>
       </c>
       <c r="B1085" s="31" t="s">
-        <v>872</v>
-      </c>
-      <c r="C1085" s="31" t="s">
-        <v>873</v>
-      </c>
-      <c r="D1085" s="31" t="s">
-        <v>873</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C1085" s="30"/>
+      <c r="D1085" s="31"/>
       <c r="E1085" s="30"/>
     </row>
     <row r="1086" spans="1:5">
@@ -19036,25 +19032,27 @@
         <v>347</v>
       </c>
       <c r="B1086" s="31" t="s">
-        <v>8</v>
+        <v>871</v>
       </c>
       <c r="C1086" s="31" t="s">
-        <v>874</v>
-      </c>
-      <c r="D1086" s="31"/>
+        <v>872</v>
+      </c>
+      <c r="D1086" s="31" t="s">
+        <v>872</v>
+      </c>
       <c r="E1086" s="30"/>
     </row>
     <row r="1087" spans="1:5">
       <c r="A1087" s="31" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B1087" s="31" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1087" s="31"/>
-      <c r="D1087" s="31" t="s">
-        <v>15</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C1087" s="31" t="s">
+        <v>873</v>
+      </c>
+      <c r="D1087" s="31"/>
       <c r="E1087" s="30"/>
     </row>
     <row r="1088" spans="1:5">
@@ -19062,12 +19060,12 @@
         <v>349</v>
       </c>
       <c r="B1088" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1088" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1088" s="31"/>
+        <v>6</v>
+      </c>
+      <c r="C1088" s="31"/>
+      <c r="D1088" s="31" t="s">
+        <v>15</v>
+      </c>
       <c r="E1088" s="30"/>
     </row>
     <row r="1089" spans="1:5">
@@ -19075,36 +19073,36 @@
         <v>349</v>
       </c>
       <c r="B1089" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1089" s="31"/>
-      <c r="D1089" s="31" t="s">
-        <v>40</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C1089" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1089" s="31"/>
       <c r="E1089" s="30"/>
     </row>
     <row r="1090" spans="1:5">
       <c r="A1090" s="31" t="s">
         <v>349</v>
       </c>
-      <c r="B1090" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1090" s="30" t="s">
-        <v>833</v>
-      </c>
-      <c r="D1090" s="30"/>
+      <c r="B1090" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1090" s="31"/>
+      <c r="D1090" s="31" t="s">
+        <v>40</v>
+      </c>
       <c r="E1090" s="30"/>
     </row>
     <row r="1091" spans="1:5">
       <c r="A1091" s="31" t="s">
         <v>349</v>
       </c>
-      <c r="B1091" s="31" t="s">
-        <v>475</v>
+      <c r="B1091" s="30" t="s">
+        <v>8</v>
       </c>
       <c r="C1091" s="30" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="D1091" s="30"/>
       <c r="E1091" s="30"/>
@@ -19113,11 +19111,11 @@
       <c r="A1092" s="31" t="s">
         <v>349</v>
       </c>
-      <c r="B1092" s="30" t="s">
-        <v>875</v>
+      <c r="B1092" s="31" t="s">
+        <v>475</v>
       </c>
       <c r="C1092" s="30" t="s">
-        <v>876</v>
+        <v>834</v>
       </c>
       <c r="D1092" s="30"/>
       <c r="E1092" s="30"/>
@@ -19127,10 +19125,10 @@
         <v>349</v>
       </c>
       <c r="B1093" s="30" t="s">
+        <v>874</v>
+      </c>
+      <c r="C1093" s="30" t="s">
         <v>875</v>
-      </c>
-      <c r="C1093" s="30" t="s">
-        <v>877</v>
       </c>
       <c r="D1093" s="30"/>
       <c r="E1093" s="30"/>
@@ -19140,10 +19138,10 @@
         <v>349</v>
       </c>
       <c r="B1094" s="30" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="C1094" s="30" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="D1094" s="30"/>
       <c r="E1094" s="30"/>
@@ -19153,10 +19151,10 @@
         <v>349</v>
       </c>
       <c r="B1095" s="30" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="C1095" s="30" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="D1095" s="30"/>
       <c r="E1095" s="30"/>
@@ -19166,186 +19164,199 @@
         <v>349</v>
       </c>
       <c r="B1096" s="30" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="C1096" s="30" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="D1096" s="30"/>
       <c r="E1096" s="30"/>
     </row>
     <row r="1097" spans="1:5">
-      <c r="A1097" s="30" t="s">
-        <v>1095</v>
-      </c>
-      <c r="B1097" s="53" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1097" s="53"/>
-      <c r="D1097" s="53" t="s">
-        <v>15</v>
-      </c>
+      <c r="A1097" s="31" t="s">
+        <v>349</v>
+      </c>
+      <c r="B1097" s="30" t="s">
+        <v>874</v>
+      </c>
+      <c r="C1097" s="30" t="s">
+        <v>879</v>
+      </c>
+      <c r="D1097" s="30"/>
       <c r="E1097" s="30"/>
     </row>
     <row r="1098" spans="1:5">
       <c r="A1098" s="30" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="B1098" s="53" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1098" s="53" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1098" s="53"/>
+        <v>6</v>
+      </c>
+      <c r="C1098" s="53"/>
+      <c r="D1098" s="53" t="s">
+        <v>15</v>
+      </c>
       <c r="E1098" s="30"/>
     </row>
     <row r="1099" spans="1:5">
       <c r="A1099" s="30" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="B1099" s="53" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C1099" s="53" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1099" s="53" t="s">
-        <v>12</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D1099" s="53"/>
       <c r="E1099" s="30"/>
     </row>
     <row r="1100" spans="1:5">
       <c r="A1100" s="30" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="B1100" s="53" t="s">
         <v>9</v>
       </c>
       <c r="C1100" s="53" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D1100" s="53" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E1100" s="30"/>
     </row>
     <row r="1101" spans="1:5">
       <c r="A1101" s="30" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="B1101" s="53" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C1101" s="53" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1101" s="53"/>
+        <v>18</v>
+      </c>
+      <c r="D1101" s="53" t="s">
+        <v>13</v>
+      </c>
       <c r="E1101" s="30"/>
     </row>
     <row r="1102" spans="1:5">
       <c r="A1102" s="30" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="B1102" s="53" t="s">
         <v>8</v>
       </c>
       <c r="C1102" s="53" t="s">
-        <v>301</v>
+        <v>19</v>
       </c>
       <c r="D1102" s="53"/>
       <c r="E1102" s="30"/>
     </row>
     <row r="1103" spans="1:5">
       <c r="A1103" s="30" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="B1103" s="53" t="s">
         <v>8</v>
       </c>
       <c r="C1103" s="53" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D1103" s="53"/>
       <c r="E1103" s="30"/>
     </row>
     <row r="1104" spans="1:5">
       <c r="A1104" s="30" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="B1104" s="53" t="s">
-        <v>308</v>
+        <v>8</v>
       </c>
       <c r="C1104" s="53" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="D1104" s="53"/>
       <c r="E1104" s="30"/>
     </row>
     <row r="1105" spans="1:5">
       <c r="A1105" s="30" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="B1105" s="53" t="s">
-        <v>8</v>
+        <v>308</v>
       </c>
       <c r="C1105" s="53" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="D1105" s="53"/>
       <c r="E1105" s="30"/>
     </row>
     <row r="1106" spans="1:5">
       <c r="A1106" s="30" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="B1106" s="53" t="s">
-        <v>148</v>
-      </c>
-      <c r="C1106" s="53"/>
-      <c r="D1106" s="53" t="s">
-        <v>1092</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C1106" s="53" t="s">
+        <v>305</v>
+      </c>
+      <c r="D1106" s="53"/>
       <c r="E1106" s="30"/>
     </row>
     <row r="1107" spans="1:5">
       <c r="A1107" s="30" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="B1107" s="53" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="C1107" s="53"/>
       <c r="D1107" s="53" t="s">
-        <v>1096</v>
+        <v>1091</v>
       </c>
       <c r="E1107" s="30"/>
     </row>
     <row r="1108" spans="1:5">
       <c r="A1108" s="30" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B1108" s="53" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1108" s="53"/>
+      <c r="D1108" s="53" t="s">
         <v>1095</v>
       </c>
-      <c r="B1108" s="53" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1108" s="53" t="s">
-        <v>128</v>
-      </c>
-      <c r="D1108" s="30"/>
       <c r="E1108" s="30"/>
     </row>
     <row r="1109" spans="1:5">
       <c r="A1109" s="30" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="B1109" s="53" t="s">
         <v>8</v>
       </c>
       <c r="C1109" s="53" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D1109" s="30"/>
       <c r="E1109" s="30"/>
+    </row>
+    <row r="1110" spans="1:5">
+      <c r="A1110" s="30" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B1110" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1110" s="53" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1110" s="30"/>
+      <c r="E1110" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19357,8 +19368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AO82"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView topLeftCell="D57" workbookViewId="0">
+      <selection activeCell="I66" sqref="I66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19373,6 +19384,7 @@
     <col min="10" max="10" width="19.42578125" customWidth="1"/>
     <col min="11" max="11" width="18.140625" customWidth="1"/>
     <col min="12" max="12" width="16.28515625" customWidth="1"/>
+    <col min="19" max="19" width="35.5703125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="60.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -19833,16 +19845,16 @@
         <v>144</v>
       </c>
       <c r="I31" s="24" t="s">
+        <v>1090</v>
+      </c>
+      <c r="J31" s="24" t="s">
         <v>1091</v>
       </c>
-      <c r="J31" s="24" t="s">
+      <c r="K31" s="24" t="s">
         <v>1092</v>
       </c>
-      <c r="K31" s="24" t="s">
+      <c r="L31" s="24" t="s">
         <v>1093</v>
-      </c>
-      <c r="L31" s="24" t="s">
-        <v>1094</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -19871,16 +19883,16 @@
         <v>147</v>
       </c>
       <c r="I32" t="s">
+        <v>1097</v>
+      </c>
+      <c r="J32" t="s">
         <v>1098</v>
       </c>
-      <c r="J32" t="s">
+      <c r="K32" t="s">
         <v>1099</v>
       </c>
-      <c r="K32" t="s">
+      <c r="L32" t="s">
         <v>1100</v>
-      </c>
-      <c r="L32" t="s">
-        <v>1101</v>
       </c>
     </row>
     <row r="33" spans="1:25">
@@ -19909,16 +19921,16 @@
         <v>147</v>
       </c>
       <c r="I33" t="s">
+        <v>1097</v>
+      </c>
+      <c r="J33" t="s">
         <v>1098</v>
       </c>
-      <c r="J33" t="s">
+      <c r="K33" t="s">
         <v>1099</v>
       </c>
-      <c r="K33" t="s">
+      <c r="L33" t="s">
         <v>1100</v>
-      </c>
-      <c r="L33" t="s">
-        <v>1101</v>
       </c>
     </row>
     <row r="35" spans="1:25">
@@ -20158,73 +20170,73 @@
         <v>4</v>
       </c>
       <c r="B49" s="36" t="s">
+        <v>880</v>
+      </c>
+      <c r="C49" s="30" t="s">
         <v>881</v>
       </c>
-      <c r="C49" s="30" t="s">
+      <c r="D49" s="37" t="s">
         <v>882</v>
       </c>
-      <c r="D49" s="37" t="s">
+      <c r="E49" s="37" t="s">
+        <v>882</v>
+      </c>
+      <c r="F49" s="30" t="s">
         <v>883</v>
       </c>
-      <c r="E49" s="37" t="s">
+      <c r="G49" s="30" t="s">
         <v>883</v>
       </c>
-      <c r="F49" s="30" t="s">
+      <c r="H49" s="30" t="s">
         <v>884</v>
       </c>
-      <c r="G49" s="30" t="s">
-        <v>884</v>
-      </c>
-      <c r="H49" s="30" t="s">
+      <c r="I49" s="38" t="s">
         <v>885</v>
       </c>
-      <c r="I49" s="38" t="s">
+      <c r="J49" s="30" t="s">
         <v>886</v>
       </c>
-      <c r="J49" s="30" t="s">
+      <c r="K49" s="30" t="s">
         <v>887</v>
       </c>
-      <c r="K49" s="30" t="s">
+      <c r="L49" s="30" t="s">
         <v>888</v>
       </c>
-      <c r="L49" s="30" t="s">
+      <c r="M49" s="30" t="s">
         <v>889</v>
       </c>
-      <c r="M49" s="30" t="s">
+      <c r="N49" t="s">
         <v>890</v>
       </c>
-      <c r="N49" t="s">
+      <c r="O49" s="30" t="s">
         <v>891</v>
       </c>
-      <c r="O49" s="30" t="s">
+      <c r="P49" s="30" t="s">
         <v>892</v>
       </c>
-      <c r="P49" s="30" t="s">
+      <c r="Q49" s="30" t="s">
         <v>893</v>
       </c>
-      <c r="Q49" s="30" t="s">
+      <c r="R49" s="30" t="s">
         <v>894</v>
       </c>
-      <c r="R49" s="30" t="s">
+      <c r="S49" s="30" t="s">
         <v>895</v>
       </c>
-      <c r="S49" s="30" t="s">
+      <c r="T49" t="s">
         <v>896</v>
       </c>
-      <c r="T49" t="s">
+      <c r="U49" s="39" t="s">
         <v>897</v>
       </c>
-      <c r="U49" s="39" t="s">
+      <c r="V49" s="39" t="s">
+        <v>897</v>
+      </c>
+      <c r="W49" t="s">
         <v>898</v>
       </c>
-      <c r="V49" s="39" t="s">
-        <v>898</v>
-      </c>
-      <c r="W49" t="s">
+      <c r="X49" s="30" t="s">
         <v>899</v>
-      </c>
-      <c r="X49" s="30" t="s">
-        <v>900</v>
       </c>
       <c r="Y49" s="30" t="s">
         <v>16</v>
@@ -20320,58 +20332,58 @@
         <v>4</v>
       </c>
       <c r="B53" s="36" t="s">
+        <v>880</v>
+      </c>
+      <c r="C53" s="30" t="s">
         <v>881</v>
       </c>
-      <c r="C53" s="30" t="s">
-        <v>882</v>
-      </c>
       <c r="D53" s="56" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="E53" s="56" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="F53" s="30" t="s">
+        <v>883</v>
+      </c>
+      <c r="G53" s="30" t="s">
+        <v>883</v>
+      </c>
+      <c r="H53" s="30" t="s">
         <v>884</v>
       </c>
-      <c r="G53" s="30" t="s">
-        <v>884</v>
-      </c>
-      <c r="H53" s="30" t="s">
-        <v>885</v>
-      </c>
       <c r="I53" s="38" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="J53" s="15" t="s">
         <v>177</v>
       </c>
       <c r="K53" s="30" t="s">
+        <v>887</v>
+      </c>
+      <c r="L53" s="30" t="s">
         <v>888</v>
       </c>
-      <c r="L53" s="30" t="s">
+      <c r="M53" s="30" t="s">
         <v>889</v>
       </c>
-      <c r="M53" s="30" t="s">
+      <c r="N53" t="s">
         <v>890</v>
       </c>
-      <c r="N53" t="s">
+      <c r="O53" s="30" t="s">
         <v>891</v>
       </c>
-      <c r="O53" s="30" t="s">
+      <c r="P53" s="30" t="s">
         <v>892</v>
       </c>
-      <c r="P53" s="30" t="s">
+      <c r="Q53" s="30" t="s">
         <v>893</v>
-      </c>
-      <c r="Q53" s="30" t="s">
-        <v>894</v>
       </c>
       <c r="R53" s="30" t="s">
         <v>16</v>
       </c>
       <c r="S53" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="54" spans="1:41">
@@ -20452,7 +20464,7 @@
         <v>634</v>
       </c>
       <c r="R56" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="S56" t="s">
         <v>646</v>
@@ -20478,73 +20490,73 @@
         <v>4</v>
       </c>
       <c r="B57" s="36" t="s">
+        <v>880</v>
+      </c>
+      <c r="C57" s="30" t="s">
         <v>881</v>
       </c>
-      <c r="C57" s="30" t="s">
-        <v>882</v>
-      </c>
       <c r="D57" s="23" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="E57" s="23" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="F57" s="30" t="s">
+        <v>883</v>
+      </c>
+      <c r="G57" s="30" t="s">
+        <v>883</v>
+      </c>
+      <c r="H57" s="30" t="s">
         <v>884</v>
       </c>
-      <c r="G57" s="30" t="s">
-        <v>884</v>
-      </c>
-      <c r="H57" s="30" t="s">
-        <v>885</v>
-      </c>
       <c r="I57" s="38" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="J57" s="41" t="s">
         <v>296</v>
       </c>
       <c r="K57" s="41" t="s">
+        <v>1101</v>
+      </c>
+      <c r="L57" s="30" t="s">
+        <v>888</v>
+      </c>
+      <c r="M57" s="30" t="s">
+        <v>889</v>
+      </c>
+      <c r="N57" t="s">
+        <v>890</v>
+      </c>
+      <c r="O57" s="30" t="s">
+        <v>891</v>
+      </c>
+      <c r="P57" s="30" t="s">
+        <v>892</v>
+      </c>
+      <c r="Q57" s="30" t="s">
+        <v>893</v>
+      </c>
+      <c r="R57" t="s">
+        <v>902</v>
+      </c>
+      <c r="S57" t="s">
+        <v>903</v>
+      </c>
+      <c r="T57" t="s">
         <v>1102</v>
       </c>
-      <c r="L57" s="30" t="s">
-        <v>889</v>
-      </c>
-      <c r="M57" s="30" t="s">
-        <v>890</v>
-      </c>
-      <c r="N57" t="s">
-        <v>891</v>
-      </c>
-      <c r="O57" s="30" t="s">
-        <v>892</v>
-      </c>
-      <c r="P57" s="30" t="s">
-        <v>893</v>
-      </c>
-      <c r="Q57" s="30" t="s">
-        <v>894</v>
-      </c>
-      <c r="R57" t="s">
-        <v>903</v>
-      </c>
-      <c r="S57" t="s">
-        <v>904</v>
-      </c>
-      <c r="T57" t="s">
+      <c r="U57" t="s">
         <v>1103</v>
       </c>
-      <c r="U57" t="s">
+      <c r="V57" t="s">
         <v>1104</v>
-      </c>
-      <c r="V57" t="s">
-        <v>1105</v>
       </c>
       <c r="W57" s="30" t="s">
         <v>16</v>
       </c>
       <c r="X57" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="58" spans="1:41">
@@ -20705,124 +20717,124 @@
         <v>4</v>
       </c>
       <c r="B62" s="36" t="s">
+        <v>904</v>
+      </c>
+      <c r="C62" s="30" t="s">
         <v>905</v>
       </c>
-      <c r="C62" s="30" t="s">
+      <c r="D62" s="37" t="s">
         <v>906</v>
       </c>
-      <c r="D62" s="37" t="s">
+      <c r="E62" s="37" t="s">
         <v>907</v>
       </c>
-      <c r="E62" s="37" t="s">
+      <c r="F62" s="30" t="s">
         <v>908</v>
       </c>
-      <c r="F62" s="30" t="s">
+      <c r="G62" s="30" t="s">
         <v>909</v>
       </c>
-      <c r="G62" s="30" t="s">
+      <c r="H62" s="30" t="s">
         <v>910</v>
       </c>
-      <c r="H62" s="30" t="s">
+      <c r="I62" s="42" t="s">
         <v>911</v>
       </c>
-      <c r="I62" s="42" t="s">
+      <c r="J62" s="30" t="s">
         <v>912</v>
       </c>
-      <c r="J62" s="30" t="s">
+      <c r="K62" t="s">
         <v>913</v>
       </c>
-      <c r="K62" t="s">
+      <c r="L62" s="30" t="s">
         <v>914</v>
       </c>
-      <c r="L62" s="30" t="s">
+      <c r="M62" t="s">
         <v>915</v>
       </c>
-      <c r="M62" t="s">
+      <c r="N62" t="s">
         <v>916</v>
       </c>
-      <c r="N62" t="s">
+      <c r="O62" s="30" t="s">
         <v>917</v>
       </c>
-      <c r="O62" s="30" t="s">
+      <c r="P62" s="37" t="s">
         <v>918</v>
       </c>
-      <c r="P62" s="37" t="s">
+      <c r="Q62" s="30" t="s">
         <v>919</v>
       </c>
-      <c r="Q62" s="30" t="s">
+      <c r="R62" s="30" t="s">
         <v>920</v>
       </c>
-      <c r="R62" s="30" t="s">
+      <c r="S62" s="43" t="s">
         <v>921</v>
       </c>
-      <c r="S62" s="43" t="s">
+      <c r="T62" s="43" t="s">
         <v>922</v>
       </c>
-      <c r="T62" s="43" t="s">
+      <c r="U62" s="30" t="s">
+        <v>886</v>
+      </c>
+      <c r="V62" s="30" t="s">
+        <v>888</v>
+      </c>
+      <c r="W62" s="30" t="s">
         <v>923</v>
       </c>
-      <c r="U62" s="30" t="s">
-        <v>887</v>
-      </c>
-      <c r="V62" s="30" t="s">
-        <v>889</v>
-      </c>
-      <c r="W62" s="30" t="s">
+      <c r="X62" s="30" t="s">
         <v>924</v>
       </c>
-      <c r="X62" s="30" t="s">
+      <c r="Y62" t="s">
+        <v>924</v>
+      </c>
+      <c r="Z62" t="s">
         <v>925</v>
       </c>
-      <c r="Y62" t="s">
-        <v>925</v>
-      </c>
-      <c r="Z62" t="s">
+      <c r="AA62" t="s">
         <v>926</v>
       </c>
-      <c r="AA62" t="s">
+      <c r="AB62" s="30" t="s">
         <v>927</v>
       </c>
-      <c r="AB62" s="30" t="s">
+      <c r="AC62" s="44" t="s">
         <v>928</v>
-      </c>
-      <c r="AC62" s="44" t="s">
-        <v>929</v>
       </c>
       <c r="AD62" s="44" t="s">
         <v>616</v>
       </c>
       <c r="AE62" s="44" t="s">
+        <v>929</v>
+      </c>
+      <c r="AF62" s="30" t="s">
         <v>930</v>
       </c>
-      <c r="AF62" s="30" t="s">
+      <c r="AG62" s="39" t="s">
         <v>931</v>
       </c>
-      <c r="AG62" s="39" t="s">
+      <c r="AH62" s="39" t="s">
         <v>932</v>
-      </c>
-      <c r="AH62" s="39" t="s">
-        <v>933</v>
       </c>
       <c r="AI62" s="15" t="s">
         <v>177</v>
       </c>
       <c r="AJ62" s="30" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="AK62" s="41" t="s">
         <v>296</v>
       </c>
       <c r="AL62" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="AM62" s="30" t="s">
         <v>16</v>
       </c>
       <c r="AN62" s="45" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="AO62" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="63" spans="1:41">
@@ -20851,25 +20863,25 @@
         <v>840</v>
       </c>
       <c r="F65" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="G65" t="s">
         <v>837</v>
       </c>
       <c r="H65" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="I65" s="40" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="J65" t="s">
+        <v>861</v>
+      </c>
+      <c r="K65" t="s">
         <v>862</v>
       </c>
-      <c r="K65" t="s">
-        <v>863</v>
-      </c>
       <c r="L65" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="M65" t="s">
         <v>839</v>
@@ -20914,28 +20926,28 @@
         <v>851</v>
       </c>
       <c r="AA65" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="AB65" s="28" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="AC65" s="46" t="s">
+        <v>937</v>
+      </c>
+      <c r="AD65" s="46" t="s">
         <v>938</v>
       </c>
-      <c r="AD65" s="46" t="s">
+      <c r="AE65" s="46" t="s">
         <v>939</v>
       </c>
-      <c r="AE65" s="46" t="s">
+      <c r="AF65" s="46" t="s">
         <v>940</v>
       </c>
-      <c r="AF65" s="46" t="s">
+      <c r="AG65" s="46" t="s">
         <v>941</v>
       </c>
-      <c r="AG65" s="46" t="s">
+      <c r="AH65" s="46" t="s">
         <v>942</v>
-      </c>
-      <c r="AH65" s="46" t="s">
-        <v>943</v>
       </c>
     </row>
     <row r="66" spans="1:34">
@@ -20943,103 +20955,103 @@
         <v>4</v>
       </c>
       <c r="B66" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="C66" t="s">
         <v>16</v>
       </c>
       <c r="D66" t="s">
+        <v>943</v>
+      </c>
+      <c r="E66" s="39" t="s">
         <v>944</v>
       </c>
-      <c r="E66" s="39" t="s">
+      <c r="F66" t="s">
         <v>945</v>
       </c>
-      <c r="F66" t="s">
+      <c r="G66" t="s">
         <v>946</v>
       </c>
-      <c r="G66" t="s">
+      <c r="H66" t="s">
         <v>947</v>
       </c>
-      <c r="H66" t="s">
+      <c r="I66" s="40" t="s">
         <v>948</v>
       </c>
-      <c r="I66" s="40" t="s">
+      <c r="J66" t="s">
         <v>949</v>
       </c>
-      <c r="J66" t="s">
+      <c r="K66" t="s">
         <v>950</v>
       </c>
-      <c r="K66" t="s">
+      <c r="L66" t="s">
         <v>951</v>
       </c>
-      <c r="L66" t="s">
+      <c r="M66" t="s">
         <v>952</v>
       </c>
-      <c r="M66" t="s">
+      <c r="N66" s="39" t="s">
         <v>953</v>
       </c>
-      <c r="N66" s="39" t="s">
+      <c r="O66" t="s">
         <v>954</v>
       </c>
-      <c r="O66" t="s">
+      <c r="P66" s="39" t="s">
         <v>955</v>
       </c>
-      <c r="P66" s="39" t="s">
+      <c r="Q66" s="39" t="s">
         <v>956</v>
       </c>
-      <c r="Q66" s="39" t="s">
+      <c r="R66" s="39" t="s">
         <v>957</v>
       </c>
-      <c r="R66" s="39" t="s">
+      <c r="S66" t="s">
         <v>958</v>
       </c>
-      <c r="S66" t="s">
+      <c r="T66" t="s">
         <v>959</v>
       </c>
-      <c r="T66" t="s">
+      <c r="U66" s="55" t="s">
         <v>960</v>
       </c>
-      <c r="U66" s="55" t="s">
+      <c r="V66" t="s">
         <v>961</v>
       </c>
-      <c r="V66" t="s">
+      <c r="W66" t="s">
         <v>962</v>
       </c>
-      <c r="W66" t="s">
+      <c r="X66" t="s">
         <v>963</v>
       </c>
-      <c r="X66" t="s">
+      <c r="Y66" s="39" t="s">
         <v>964</v>
       </c>
-      <c r="Y66" s="39" t="s">
+      <c r="Z66" s="39" t="s">
         <v>965</v>
       </c>
-      <c r="Z66" s="39" t="s">
+      <c r="AA66" t="s">
         <v>966</v>
       </c>
-      <c r="AA66" t="s">
+      <c r="AB66" t="s">
         <v>967</v>
       </c>
-      <c r="AB66" t="s">
+      <c r="AC66" s="39" t="s">
         <v>968</v>
       </c>
-      <c r="AC66" s="39" t="s">
+      <c r="AD66" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="AD66" s="39" t="s">
+      <c r="AE66" s="39" t="s">
         <v>970</v>
       </c>
-      <c r="AE66" s="39" t="s">
+      <c r="AF66" s="39" t="s">
         <v>971</v>
       </c>
-      <c r="AF66" s="39" t="s">
+      <c r="AG66" t="s">
         <v>972</v>
       </c>
-      <c r="AG66" t="s">
+      <c r="AH66" s="39" t="s">
         <v>973</v>
-      </c>
-      <c r="AH66" s="39" t="s">
-        <v>974</v>
       </c>
     </row>
     <row r="67" spans="1:34">
@@ -21104,7 +21116,7 @@
         <v>851</v>
       </c>
       <c r="R69" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="S69" s="28" t="s">
         <v>840</v>
@@ -21115,58 +21127,58 @@
         <v>4</v>
       </c>
       <c r="B70" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="C70" t="s">
         <v>16</v>
       </c>
       <c r="D70" t="s">
+        <v>952</v>
+      </c>
+      <c r="E70" s="39" t="s">
         <v>953</v>
       </c>
-      <c r="E70" s="39" t="s">
+      <c r="F70" t="s">
         <v>954</v>
       </c>
-      <c r="F70" t="s">
+      <c r="G70" s="39" t="s">
         <v>955</v>
       </c>
-      <c r="G70" s="39" t="s">
+      <c r="H70" s="39" t="s">
         <v>956</v>
       </c>
-      <c r="H70" s="39" t="s">
+      <c r="I70" s="39" t="s">
         <v>957</v>
       </c>
-      <c r="I70" s="39" t="s">
+      <c r="J70" t="s">
         <v>958</v>
       </c>
-      <c r="J70" t="s">
+      <c r="K70" t="s">
         <v>959</v>
       </c>
-      <c r="K70" t="s">
+      <c r="L70" s="39" t="s">
         <v>960</v>
       </c>
-      <c r="L70" s="39" t="s">
+      <c r="M70" t="s">
         <v>961</v>
       </c>
-      <c r="M70" t="s">
+      <c r="N70" t="s">
         <v>962</v>
       </c>
-      <c r="N70" t="s">
+      <c r="O70" t="s">
         <v>963</v>
       </c>
-      <c r="O70" t="s">
+      <c r="P70" s="39" t="s">
         <v>964</v>
       </c>
-      <c r="P70" s="39" t="s">
+      <c r="Q70" s="39" t="s">
         <v>965</v>
       </c>
-      <c r="Q70" s="39" t="s">
+      <c r="R70" t="s">
         <v>966</v>
       </c>
-      <c r="R70" t="s">
-        <v>967</v>
-      </c>
       <c r="S70" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="71" spans="1:34">
@@ -21189,25 +21201,25 @@
         <v>15</v>
       </c>
       <c r="D73" s="46" t="s">
+        <v>937</v>
+      </c>
+      <c r="E73" s="46" t="s">
         <v>938</v>
       </c>
-      <c r="E73" s="46" t="s">
+      <c r="F73" s="46" t="s">
         <v>939</v>
       </c>
-      <c r="F73" s="46" t="s">
+      <c r="G73" s="46" t="s">
         <v>940</v>
       </c>
-      <c r="G73" s="46" t="s">
+      <c r="H73" s="46" t="s">
         <v>941</v>
       </c>
-      <c r="H73" s="46" t="s">
+      <c r="I73" s="46" t="s">
         <v>942</v>
       </c>
-      <c r="I73" s="46" t="s">
-        <v>943</v>
-      </c>
       <c r="J73" s="28" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="74" spans="1:34">
@@ -21215,31 +21227,31 @@
         <v>4</v>
       </c>
       <c r="B74" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="C74" t="s">
         <v>16</v>
       </c>
       <c r="D74" s="39" t="s">
+        <v>968</v>
+      </c>
+      <c r="E74" s="39" t="s">
+        <v>945</v>
+      </c>
+      <c r="F74" s="39" t="s">
+        <v>970</v>
+      </c>
+      <c r="G74" s="39" t="s">
         <v>969</v>
       </c>
-      <c r="E74" s="39" t="s">
-        <v>946</v>
-      </c>
-      <c r="F74" s="39" t="s">
+      <c r="H74" s="39" t="s">
         <v>971</v>
       </c>
-      <c r="G74" s="39" t="s">
-        <v>970</v>
-      </c>
-      <c r="H74" s="39" t="s">
-        <v>972</v>
-      </c>
       <c r="I74" s="39" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="J74" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="75" spans="1:34">
@@ -21277,13 +21289,13 @@
         <v>16</v>
       </c>
       <c r="D78" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="I78" s="40"/>
     </row>
     <row r="80" spans="1:34">
       <c r="A80" s="19" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -21300,10 +21312,10 @@
         <v>13</v>
       </c>
       <c r="E81" s="24" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="F81" s="24" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -21320,10 +21332,10 @@
         <v>126</v>
       </c>
       <c r="E82" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="F82" s="15" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
   </sheetData>
@@ -21960,7 +21972,7 @@
     </row>
     <row r="15" spans="1:47" s="3" customFormat="1" ht="28.5" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="AJ15" s="48"/>
     </row>
@@ -22177,19 +22189,19 @@
         <v>461</v>
       </c>
       <c r="AK20" s="1" t="s">
+        <v>978</v>
+      </c>
+      <c r="AL20" s="1" t="s">
         <v>979</v>
       </c>
-      <c r="AL20" s="1" t="s">
+      <c r="AM20" s="1" t="s">
         <v>980</v>
-      </c>
-      <c r="AM20" s="1" t="s">
-        <v>981</v>
       </c>
       <c r="AN20" s="1" t="s">
         <v>15</v>
       </c>
       <c r="AO20" s="1" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="AP20" s="1" t="s">
         <v>392</v>
@@ -22201,7 +22213,7 @@
         <v>419</v>
       </c>
       <c r="AS20" s="22" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="AT20" s="22" t="s">
         <v>454</v>
@@ -22227,145 +22239,145 @@
         <v>44</v>
       </c>
       <c r="C21" t="s">
+        <v>983</v>
+      </c>
+      <c r="D21" t="s">
         <v>984</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>985</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>986</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>987</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>988</v>
-      </c>
-      <c r="H21" t="s">
-        <v>989</v>
       </c>
       <c r="I21" t="s">
         <v>225</v>
       </c>
       <c r="J21" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="K21" t="s">
+        <v>989</v>
+      </c>
+      <c r="L21" s="14" t="s">
         <v>990</v>
       </c>
-      <c r="L21" s="14" t="s">
+      <c r="M21" s="14" t="s">
         <v>991</v>
       </c>
-      <c r="M21" s="14" t="s">
+      <c r="N21" t="s">
         <v>992</v>
       </c>
-      <c r="N21" t="s">
+      <c r="O21" t="s">
         <v>993</v>
       </c>
-      <c r="O21" t="s">
+      <c r="P21" s="39" t="s">
         <v>994</v>
       </c>
-      <c r="P21" s="39" t="s">
+      <c r="Q21" t="s">
         <v>995</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="R21" s="39" t="s">
         <v>996</v>
       </c>
-      <c r="R21" s="39" t="s">
+      <c r="S21" s="15" t="s">
         <v>997</v>
       </c>
-      <c r="S21" s="15" t="s">
+      <c r="T21" t="s">
         <v>998</v>
       </c>
-      <c r="T21" t="s">
+      <c r="U21" t="s">
         <v>999</v>
       </c>
-      <c r="U21" t="s">
+      <c r="V21" s="39" t="s">
         <v>1000</v>
       </c>
-      <c r="V21" s="39" t="s">
+      <c r="W21" s="15" t="s">
         <v>1001</v>
       </c>
-      <c r="W21" s="15" t="s">
+      <c r="X21" s="39" t="s">
         <v>1002</v>
       </c>
-      <c r="X21" s="39" t="s">
+      <c r="Y21" t="s">
         <v>1003</v>
       </c>
-      <c r="Y21" t="s">
+      <c r="Z21" s="39" t="s">
         <v>1004</v>
       </c>
-      <c r="Z21" s="39" t="s">
+      <c r="AA21" s="15" t="s">
         <v>1005</v>
-      </c>
-      <c r="AA21" s="15" t="s">
-        <v>1006</v>
       </c>
       <c r="AB21" s="15" t="s">
         <v>109</v>
       </c>
       <c r="AC21" s="39" t="s">
+        <v>1006</v>
+      </c>
+      <c r="AD21" t="s">
         <v>1007</v>
       </c>
-      <c r="AD21" t="s">
+      <c r="AE21" t="s">
+        <v>891</v>
+      </c>
+      <c r="AF21" t="s">
         <v>1008</v>
       </c>
-      <c r="AE21" t="s">
-        <v>892</v>
-      </c>
-      <c r="AF21" t="s">
+      <c r="AG21" t="s">
+        <v>890</v>
+      </c>
+      <c r="AH21" t="s">
         <v>1009</v>
       </c>
-      <c r="AG21" t="s">
-        <v>891</v>
-      </c>
-      <c r="AH21" t="s">
+      <c r="AI21" t="s">
         <v>1010</v>
       </c>
-      <c r="AI21" t="s">
+      <c r="AJ21" s="4" t="s">
         <v>1011</v>
       </c>
-      <c r="AJ21" s="4" t="s">
+      <c r="AK21" s="4" t="s">
         <v>1012</v>
       </c>
-      <c r="AK21" s="4" t="s">
+      <c r="AL21" t="s">
         <v>1013</v>
       </c>
-      <c r="AL21" t="s">
+      <c r="AM21" t="s">
         <v>1014</v>
-      </c>
-      <c r="AM21" t="s">
-        <v>1015</v>
       </c>
       <c r="AN21" t="s">
         <v>16</v>
       </c>
       <c r="AO21" t="s">
+        <v>1015</v>
+      </c>
+      <c r="AP21" t="s">
         <v>1016</v>
       </c>
-      <c r="AP21" t="s">
+      <c r="AQ21" t="s">
         <v>1017</v>
       </c>
-      <c r="AQ21" t="s">
+      <c r="AR21" t="s">
         <v>1018</v>
       </c>
-      <c r="AR21" t="s">
+      <c r="AS21" t="s">
         <v>1019</v>
       </c>
-      <c r="AS21" t="s">
+      <c r="AT21" t="s">
         <v>1020</v>
       </c>
-      <c r="AT21" t="s">
+      <c r="AU21" t="s">
         <v>1021</v>
-      </c>
-      <c r="AU21" t="s">
-        <v>1022</v>
       </c>
       <c r="AV21" t="s">
         <v>16</v>
       </c>
       <c r="AW21" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="AX21" t="s">
         <v>267</v>
@@ -22565,130 +22577,130 @@
         <v>42</v>
       </c>
       <c r="C25" t="s">
+        <v>1023</v>
+      </c>
+      <c r="D25" t="s">
         <v>1024</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>1025</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>1026</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>1027</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" s="39" t="s">
         <v>1028</v>
       </c>
-      <c r="H25" s="39" t="s">
+      <c r="I25" t="s">
+        <v>891</v>
+      </c>
+      <c r="J25" t="s">
+        <v>1008</v>
+      </c>
+      <c r="K25" t="s">
+        <v>890</v>
+      </c>
+      <c r="L25" t="s">
+        <v>1009</v>
+      </c>
+      <c r="M25" t="s">
         <v>1029</v>
       </c>
-      <c r="I25" t="s">
-        <v>892</v>
-      </c>
-      <c r="J25" t="s">
-        <v>1009</v>
-      </c>
-      <c r="K25" t="s">
-        <v>891</v>
-      </c>
-      <c r="L25" t="s">
-        <v>1010</v>
-      </c>
-      <c r="M25" t="s">
+      <c r="N25" t="s">
         <v>1030</v>
       </c>
-      <c r="N25" t="s">
+      <c r="O25" t="s">
         <v>1031</v>
       </c>
-      <c r="O25" t="s">
+      <c r="P25" t="s">
         <v>1032</v>
       </c>
-      <c r="P25" t="s">
+      <c r="Q25" t="s">
         <v>1033</v>
       </c>
-      <c r="Q25" t="s">
+      <c r="R25" t="s">
         <v>1034</v>
       </c>
-      <c r="R25" t="s">
+      <c r="S25" t="s">
         <v>1035</v>
       </c>
-      <c r="S25" t="s">
+      <c r="T25" t="s">
         <v>1036</v>
-      </c>
-      <c r="T25" t="s">
-        <v>1037</v>
       </c>
       <c r="U25" t="s">
         <v>534</v>
       </c>
       <c r="V25" s="39" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="W25" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="X25" t="s">
         <v>540</v>
       </c>
       <c r="Y25" s="39" t="s">
+        <v>1038</v>
+      </c>
+      <c r="Z25" t="s">
         <v>1039</v>
-      </c>
-      <c r="Z25" t="s">
-        <v>1040</v>
       </c>
       <c r="AA25" t="s">
         <v>546</v>
       </c>
       <c r="AB25" s="39" t="s">
+        <v>1040</v>
+      </c>
+      <c r="AC25" t="s">
         <v>1041</v>
-      </c>
-      <c r="AC25" t="s">
-        <v>1042</v>
       </c>
       <c r="AD25" t="s">
         <v>552</v>
       </c>
       <c r="AE25" s="39" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="AF25">
         <v>100000</v>
       </c>
       <c r="AG25" s="39" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="AH25" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="AI25" t="s">
+        <v>1008</v>
+      </c>
+      <c r="AJ25" t="s">
+        <v>890</v>
+      </c>
+      <c r="AK25" t="s">
         <v>1009</v>
-      </c>
-      <c r="AJ25" t="s">
-        <v>891</v>
-      </c>
-      <c r="AK25" t="s">
-        <v>1010</v>
       </c>
       <c r="AV25" t="s">
         <v>16</v>
       </c>
       <c r="AW25" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="AX25" t="s">
+        <v>1044</v>
+      </c>
+      <c r="AY25" t="s">
         <v>1045</v>
       </c>
-      <c r="AY25" t="s">
+      <c r="AZ25" t="s">
         <v>1046</v>
       </c>
-      <c r="AZ25" t="s">
+      <c r="BA25" t="s">
         <v>1047</v>
       </c>
-      <c r="BA25" t="s">
+      <c r="BB25" t="s">
         <v>1048</v>
-      </c>
-      <c r="BB25" t="s">
-        <v>1049</v>
       </c>
     </row>
     <row r="26" spans="1:56">
@@ -22791,37 +22803,37 @@
         <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="C29" t="s">
         <v>161</v>
       </c>
       <c r="D29" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="E29" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="F29" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="G29" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="H29" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="I29" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="J29" t="s">
+        <v>1050</v>
+      </c>
+      <c r="K29" t="s">
         <v>1051</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" t="s">
         <v>1052</v>
-      </c>
-      <c r="L29" t="s">
-        <v>1053</v>
       </c>
       <c r="M29" t="s">
         <v>16</v>
@@ -23013,19 +23025,19 @@
         <v>16</v>
       </c>
       <c r="D33" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="E33" t="s">
         <v>116</v>
       </c>
       <c r="F33" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="G33" t="s">
         <v>117</v>
       </c>
       <c r="H33" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="I33" t="s">
         <v>118</v>
@@ -23040,40 +23052,40 @@
         <v>121</v>
       </c>
       <c r="M33" s="39" t="s">
+        <v>1056</v>
+      </c>
+      <c r="N33" s="15" t="s">
+        <v>997</v>
+      </c>
+      <c r="O33" s="15" t="s">
         <v>1057</v>
-      </c>
-      <c r="N33" s="15" t="s">
-        <v>998</v>
-      </c>
-      <c r="O33" s="15" t="s">
-        <v>1058</v>
       </c>
       <c r="P33" t="s">
         <v>161</v>
       </c>
       <c r="Q33" t="s">
+        <v>1058</v>
+      </c>
+      <c r="R33" t="s">
         <v>1059</v>
       </c>
-      <c r="R33" t="s">
+      <c r="S33" t="s">
         <v>1060</v>
       </c>
-      <c r="S33" t="s">
+      <c r="T33" t="s">
         <v>1061</v>
       </c>
-      <c r="T33" t="s">
+      <c r="U33" t="s">
         <v>1062</v>
-      </c>
-      <c r="U33" t="s">
-        <v>1063</v>
       </c>
       <c r="V33" t="s">
         <v>161</v>
       </c>
       <c r="W33" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="X33" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="Y33">
         <v>11</v>
@@ -23236,16 +23248,16 @@
         <v>161</v>
       </c>
       <c r="E37" t="s">
+        <v>1064</v>
+      </c>
+      <c r="F37" t="s">
+        <v>1058</v>
+      </c>
+      <c r="G37" s="39" t="s">
         <v>1065</v>
       </c>
-      <c r="F37" t="s">
-        <v>1059</v>
-      </c>
-      <c r="G37" s="39" t="s">
-        <v>1066</v>
-      </c>
       <c r="H37" s="39" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="I37">
         <v>22</v>
@@ -23284,7 +23296,7 @@
         <v>44</v>
       </c>
       <c r="U37" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="AJ37" s="4"/>
     </row>
@@ -23444,82 +23456,82 @@
         <v>16</v>
       </c>
       <c r="D41" t="s">
+        <v>1067</v>
+      </c>
+      <c r="E41" t="s">
         <v>1068</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>1069</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>1070</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>1071</v>
       </c>
-      <c r="H41" t="s">
+      <c r="I41" t="s">
         <v>1072</v>
       </c>
-      <c r="I41" t="s">
+      <c r="J41" t="s">
         <v>1073</v>
       </c>
-      <c r="J41" t="s">
+      <c r="K41" t="s">
         <v>1074</v>
       </c>
-      <c r="K41" t="s">
+      <c r="L41" t="s">
         <v>1075</v>
       </c>
-      <c r="L41" t="s">
+      <c r="M41" t="s">
         <v>1076</v>
       </c>
-      <c r="M41" t="s">
+      <c r="N41" t="s">
         <v>1077</v>
       </c>
-      <c r="N41" t="s">
+      <c r="O41" t="s">
         <v>1078</v>
       </c>
-      <c r="O41" t="s">
+      <c r="P41" t="s">
         <v>1079</v>
       </c>
-      <c r="P41" t="s">
+      <c r="Q41" s="15" t="s">
+        <v>997</v>
+      </c>
+      <c r="R41" t="s">
         <v>1080</v>
       </c>
-      <c r="Q41" s="15" t="s">
-        <v>998</v>
-      </c>
-      <c r="R41" t="s">
+      <c r="S41" t="s">
         <v>1081</v>
       </c>
-      <c r="S41" t="s">
+      <c r="T41" t="s">
         <v>1082</v>
       </c>
-      <c r="T41" t="s">
+      <c r="U41" t="s">
         <v>1083</v>
-      </c>
-      <c r="U41" t="s">
-        <v>1084</v>
       </c>
       <c r="V41" t="s">
         <v>267</v>
       </c>
       <c r="W41" t="s">
+        <v>1084</v>
+      </c>
+      <c r="X41" t="s">
         <v>1085</v>
       </c>
-      <c r="X41" t="s">
+      <c r="Y41" t="s">
         <v>1086</v>
       </c>
-      <c r="Y41" t="s">
+      <c r="Z41" t="s">
         <v>1087</v>
       </c>
-      <c r="Z41" t="s">
+      <c r="AA41" t="s">
         <v>1088</v>
       </c>
-      <c r="AA41" t="s">
+      <c r="AB41" t="s">
         <v>1089</v>
       </c>
-      <c r="AB41" t="s">
-        <v>1090</v>
-      </c>
       <c r="AC41" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="AD41" t="s">
         <v>162</v>

</xml_diff>

<commit_message>
Moving Sai's changes in excel to github
</commit_message>
<xml_diff>
--- a/src/com/supplierconnection/xls/TestSuite1.xlsx
+++ b/src/com/supplierconnection/xls/TestSuite1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12315" windowHeight="2055"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12315" windowHeight="2055" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6604" uniqueCount="1405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6932" uniqueCount="1483">
   <si>
     <t>TCID</t>
   </si>
@@ -4260,11 +4260,245 @@
   <si>
     <t>Checking bookmark active/inactive in saved bookmark</t>
   </si>
+  <si>
+    <t>Events</t>
+  </si>
+  <si>
+    <t>SavedSearch</t>
+  </si>
+  <si>
+    <t>OpportunityPost</t>
+  </si>
+  <si>
+    <t>eventsText</t>
+  </si>
+  <si>
+    <t>Expected Data</t>
+  </si>
+  <si>
+    <t>suggestAnEvent</t>
+  </si>
+  <si>
+    <t>suggestAnEven_text_onThePage</t>
+  </si>
+  <si>
+    <t>Expected Data_Events_Overlay</t>
+  </si>
+  <si>
+    <t>eventTitle</t>
+  </si>
+  <si>
+    <t>Event_Title_Input</t>
+  </si>
+  <si>
+    <t>Website_Input</t>
+  </si>
+  <si>
+    <t>eventHashtag</t>
+  </si>
+  <si>
+    <t>EventHashtag_Input</t>
+  </si>
+  <si>
+    <t>eventCity</t>
+  </si>
+  <si>
+    <t>Event_City</t>
+  </si>
+  <si>
+    <t>Select_State</t>
+  </si>
+  <si>
+    <t>startMonth</t>
+  </si>
+  <si>
+    <t>Start_Month</t>
+  </si>
+  <si>
+    <t>startDay</t>
+  </si>
+  <si>
+    <t>Start_Day</t>
+  </si>
+  <si>
+    <t>startYear</t>
+  </si>
+  <si>
+    <t>Start_Year</t>
+  </si>
+  <si>
+    <t>endMonth</t>
+  </si>
+  <si>
+    <t>End_Month</t>
+  </si>
+  <si>
+    <t>endDay</t>
+  </si>
+  <si>
+    <t>End_Day</t>
+  </si>
+  <si>
+    <t>endYear</t>
+  </si>
+  <si>
+    <t>End_Year</t>
+  </si>
+  <si>
+    <t>IBM_checkBox</t>
+  </si>
+  <si>
+    <t>PRIVATE_NOTE_TO_THE_EVENT_REVIEWER</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>eventPage_submitBtn</t>
+  </si>
+  <si>
+    <t>thanks_event_submitPage</t>
+  </si>
+  <si>
+    <t>Text_in_Event_Submit_Page</t>
+  </si>
+  <si>
+    <t>submit_btn</t>
+  </si>
+  <si>
+    <t>searchSuppliersSearchBox</t>
+  </si>
+  <si>
+    <t>searchIcon</t>
+  </si>
+  <si>
+    <t>saveSearch</t>
+  </si>
+  <si>
+    <t>nameYourSrch</t>
+  </si>
+  <si>
+    <t>searchName</t>
+  </si>
+  <si>
+    <t>saveBtnSavSrch</t>
+  </si>
+  <si>
+    <t>mySSAlertsOppP</t>
+  </si>
+  <si>
+    <t>dropdownArrow</t>
+  </si>
+  <si>
+    <t>old2New</t>
+  </si>
+  <si>
+    <t>searchNamePresent</t>
+  </si>
+  <si>
+    <t>selectBySrchTxt</t>
+  </si>
+  <si>
+    <t>activeDays</t>
+  </si>
+  <si>
+    <t>daysActive</t>
+  </si>
+  <si>
+    <t>postTitle</t>
+  </si>
+  <si>
+    <t>postDesc</t>
+  </si>
+  <si>
+    <t>welcomeTab</t>
+  </si>
+  <si>
+    <t>opportunityMarketPlaceLink</t>
+  </si>
+  <si>
+    <t>op_title</t>
+  </si>
+  <si>
+    <t>opTitle</t>
+  </si>
+  <si>
+    <t>moveToElement</t>
+  </si>
+  <si>
+    <t>op_element</t>
+  </si>
+  <si>
+    <t>Expected Data_BuyerAdmin Page</t>
+  </si>
+  <si>
+    <t>Suggest an event</t>
+  </si>
+  <si>
+    <t>May 12 16</t>
+  </si>
+  <si>
+    <t>http://gmail.com</t>
+  </si>
+  <si>
+    <t>PARTY</t>
+  </si>
+  <si>
+    <t>Bengaluru</t>
+  </si>
+  <si>
+    <t>North Carolina</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>Thank you for your suggestion. Your event has been submitted for review.</t>
+  </si>
+  <si>
+    <t>searchTxtVerification</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>Automotive</t>
+  </si>
+  <si>
+    <t>IBMIndiaBlr2</t>
+  </si>
+  <si>
+    <t>saikrishna@ibm.com</t>
+  </si>
+  <si>
+    <t>postInfo</t>
+  </si>
+  <si>
+    <t>15 Days</t>
+  </si>
+  <si>
+    <t>Sai_postTitle</t>
+  </si>
+  <si>
+    <t>Description : This is testing</t>
+  </si>
+  <si>
+    <t>Opportunity Marketplace</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
@@ -4481,7 +4715,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -4578,6 +4812,16 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4672,6 +4916,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -4707,6 +4968,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4883,10 +5161,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:C32"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:XFD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5247,6 +5525,30 @@
         <v>4</v>
       </c>
     </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1406</v>
+      </c>
+      <c r="C34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>1407</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5254,10 +5556,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1531"/>
+  <dimension ref="A1:G1610"/>
   <sheetViews>
-    <sheetView topLeftCell="A1511" workbookViewId="0">
-      <selection activeCell="A1519" sqref="A1519:D1531"/>
+    <sheetView topLeftCell="A1516" workbookViewId="0">
+      <selection activeCell="A1532" sqref="A1532:D1610"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24043,6 +24345,926 @@
         <v>1120</v>
       </c>
     </row>
+    <row r="1532" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1532" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B1532" s="64" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1532" s="64"/>
+      <c r="D1532" s="64" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1533" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1533" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B1533" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1533" s="64" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1533" s="64"/>
+    </row>
+    <row r="1534" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1534" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B1534" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1534" s="74"/>
+      <c r="D1534" s="74" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="1535" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1535" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B1535" t="s">
+        <v>481</v>
+      </c>
+      <c r="C1535" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="1536" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1536" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B1536" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1536" t="s">
+        <v>1408</v>
+      </c>
+      <c r="D1536" t="s">
+        <v>1409</v>
+      </c>
+    </row>
+    <row r="1537" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1537" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B1537" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1537" s="74" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="1538" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1538" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B1538" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1538" s="74" t="s">
+        <v>1411</v>
+      </c>
+      <c r="D1538" t="s">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="1539" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1539" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B1539" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1539" s="74" t="s">
+        <v>1413</v>
+      </c>
+      <c r="D1539" t="s">
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="1540" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1540" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B1540" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1540" s="74" t="s">
+        <v>498</v>
+      </c>
+      <c r="D1540" t="s">
+        <v>1415</v>
+      </c>
+    </row>
+    <row r="1541" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1541" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B1541" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1541" s="74" t="s">
+        <v>1416</v>
+      </c>
+      <c r="D1541" t="s">
+        <v>1417</v>
+      </c>
+    </row>
+    <row r="1542" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1542" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B1542" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1542" s="74" t="s">
+        <v>1418</v>
+      </c>
+      <c r="D1542" t="s">
+        <v>1419</v>
+      </c>
+    </row>
+    <row r="1543" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1543" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B1543" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1543" s="74" t="s">
+        <v>382</v>
+      </c>
+      <c r="D1543" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="1544" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1544" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B1544" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1544" t="s">
+        <v>1421</v>
+      </c>
+      <c r="D1544" t="s">
+        <v>1422</v>
+      </c>
+    </row>
+    <row r="1545" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1545" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B1545" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1545" t="s">
+        <v>1423</v>
+      </c>
+      <c r="D1545" t="s">
+        <v>1424</v>
+      </c>
+    </row>
+    <row r="1546" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1546" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B1546" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1546" t="s">
+        <v>1425</v>
+      </c>
+      <c r="D1546" t="s">
+        <v>1426</v>
+      </c>
+    </row>
+    <row r="1547" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1547" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B1547" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1547" t="s">
+        <v>1427</v>
+      </c>
+      <c r="D1547" t="s">
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="1548" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1548" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B1548" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1548" t="s">
+        <v>1429</v>
+      </c>
+      <c r="D1548" t="s">
+        <v>1430</v>
+      </c>
+    </row>
+    <row r="1549" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1549" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B1549" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1549" t="s">
+        <v>1431</v>
+      </c>
+      <c r="D1549" t="s">
+        <v>1432</v>
+      </c>
+    </row>
+    <row r="1550" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1550" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B1550" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1550" t="s">
+        <v>1433</v>
+      </c>
+    </row>
+    <row r="1551" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1551" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B1551" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1551" t="s">
+        <v>1434</v>
+      </c>
+      <c r="D1551" t="s">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="1552" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1552" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B1552" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1552" t="s">
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="1553" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1553" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B1553" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1553" t="s">
+        <v>1437</v>
+      </c>
+      <c r="D1553" t="s">
+        <v>1438</v>
+      </c>
+    </row>
+    <row r="1554" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1554" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B1554" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1554" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="1555" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1555" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B1555" s="64" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1555" s="64"/>
+      <c r="D1555" s="64" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1556" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1556" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B1556" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1556" s="64" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1556" s="64"/>
+    </row>
+    <row r="1557" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1557" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B1557" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1557" s="74"/>
+      <c r="D1557" s="74" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="1558" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1558" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B1558" t="s">
+        <v>481</v>
+      </c>
+      <c r="C1558" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="1559" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1559" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B1559" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1559" t="s">
+        <v>1408</v>
+      </c>
+      <c r="D1559" t="s">
+        <v>1409</v>
+      </c>
+    </row>
+    <row r="1560" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1560" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B1560" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1560" s="74" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="1561" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1561" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B1561" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1561" s="74" t="s">
+        <v>1411</v>
+      </c>
+      <c r="D1561" t="s">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="1562" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1562" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B1562" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1562" t="s">
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="1563" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1563" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B1563" s="64" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1563" s="64"/>
+      <c r="D1563" s="64" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1564" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1564" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B1564" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1564" s="64" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1564" s="64"/>
+    </row>
+    <row r="1565" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1565" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B1565" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1565" s="74"/>
+      <c r="D1565" s="74" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="1566" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1566" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B1566" t="s">
+        <v>481</v>
+      </c>
+      <c r="C1566" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="1567" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1567" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B1567" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1567" t="s">
+        <v>1440</v>
+      </c>
+      <c r="D1567" t="s">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="1568" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1568" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B1568" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1568" t="s">
+        <v>1441</v>
+      </c>
+    </row>
+    <row r="1569" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1569" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B1569" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1570" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1570" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B1570" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1570" t="s">
+        <v>1440</v>
+      </c>
+      <c r="D1570" t="s">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="1571" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1571" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B1571" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1571" t="s">
+        <v>1442</v>
+      </c>
+    </row>
+    <row r="1572" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1572" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B1572" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1573" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1573" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B1573" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1573" t="s">
+        <v>1443</v>
+      </c>
+      <c r="D1573" t="s">
+        <v>1444</v>
+      </c>
+    </row>
+    <row r="1574" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1574" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B1574" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1575" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1575" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B1575" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1575" t="s">
+        <v>1445</v>
+      </c>
+    </row>
+    <row r="1576" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1576" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B1576" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1577" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1577" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B1577" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1577" t="s">
+        <v>1446</v>
+      </c>
+    </row>
+    <row r="1578" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1578" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B1578" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1579" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1579" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B1579" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1579" t="s">
+        <v>1447</v>
+      </c>
+    </row>
+    <row r="1580" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1580" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B1580" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1581" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1581" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B1581" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1581" t="s">
+        <v>1448</v>
+      </c>
+    </row>
+    <row r="1582" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1582" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B1582" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1582" t="s">
+        <v>1449</v>
+      </c>
+      <c r="D1582" t="s">
+        <v>1444</v>
+      </c>
+    </row>
+    <row r="1583" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1583" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B1583" t="s">
+        <v>481</v>
+      </c>
+      <c r="C1583" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="1584" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1584" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B1584" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1585" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1585" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B1585" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1585" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="1586" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1586" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B1586" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1586" t="s">
+        <v>1450</v>
+      </c>
+      <c r="D1586" t="s">
+        <v>1444</v>
+      </c>
+    </row>
+    <row r="1587" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1587" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B1587" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1588" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1588" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B1588" s="64" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1588" s="64"/>
+      <c r="D1588" s="64" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1589" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1589" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B1589" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1589" s="64" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1589" s="64"/>
+    </row>
+    <row r="1590" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1590" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B1590" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1590" s="74"/>
+      <c r="D1590" s="74" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="1591" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1591" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B1591" t="s">
+        <v>481</v>
+      </c>
+      <c r="C1591" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="1592" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1592" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B1592" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1592" t="s">
+        <v>1440</v>
+      </c>
+      <c r="D1592" t="s">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="1593" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1593" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B1593" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1593" t="s">
+        <v>1441</v>
+      </c>
+    </row>
+    <row r="1594" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1594" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B1594" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1595" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1595" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B1595" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1595" t="s">
+        <v>1442</v>
+      </c>
+    </row>
+    <row r="1596" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1596" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B1596" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1597" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1597" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B1597" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1597" t="s">
+        <v>1443</v>
+      </c>
+      <c r="D1597" t="s">
+        <v>1444</v>
+      </c>
+    </row>
+    <row r="1598" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1598" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B1598" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1598" t="s">
+        <v>1451</v>
+      </c>
+      <c r="D1598" t="s">
+        <v>1452</v>
+      </c>
+    </row>
+    <row r="1599" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1599" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B1599" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1599" t="s">
+        <v>1453</v>
+      </c>
+      <c r="D1599" t="s">
+        <v>1453</v>
+      </c>
+    </row>
+    <row r="1600" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1600" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B1600" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1600" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D1600" t="s">
+        <v>1454</v>
+      </c>
+    </row>
+    <row r="1601" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1601" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B1601" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1601" t="s">
+        <v>1445</v>
+      </c>
+    </row>
+    <row r="1602" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1602" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B1602" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1603" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1603" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B1603" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1603" t="s">
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="1604" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1604" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B1604" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1605" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1605" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B1605" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1605" t="s">
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="1606" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1606" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B1606" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1607" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1607" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B1607" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1608" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1608" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B1608" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1608" t="s">
+        <v>1457</v>
+      </c>
+      <c r="D1608" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="1609" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1609" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B1609" t="s">
+        <v>1459</v>
+      </c>
+      <c r="C1609" t="s">
+        <v>1460</v>
+      </c>
+    </row>
+    <row r="1610" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1610" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B1610" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -24051,10 +25273,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO124"/>
+  <dimension ref="A1:AO136"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="A119" sqref="A119:A124"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="A126" sqref="A126:XFD136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26795,7 +28017,7 @@
         <v>1392</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>4</v>
       </c>
@@ -26809,7 +28031,7 @@
         <v>1393</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>4</v>
       </c>
@@ -26823,12 +28045,12 @@
         <v>1393</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A116" s="21" t="s">
         <v>1116</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>14</v>
       </c>
@@ -26851,7 +28073,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>4</v>
       </c>
@@ -26874,7 +28096,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>4</v>
       </c>
@@ -26897,7 +28119,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>4</v>
       </c>
@@ -26920,7 +28142,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>4</v>
       </c>
@@ -26943,7 +28165,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>4</v>
       </c>
@@ -26966,7 +28188,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>4</v>
       </c>
@@ -26989,7 +28211,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>4</v>
       </c>
@@ -27010,6 +28232,257 @@
       </c>
       <c r="G124" t="s">
         <v>1118</v>
+      </c>
+    </row>
+    <row r="126" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>1405</v>
+      </c>
+      <c r="I126" s="49"/>
+    </row>
+    <row r="127" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>14</v>
+      </c>
+      <c r="B127" t="s">
+        <v>40</v>
+      </c>
+      <c r="C127" t="s">
+        <v>15</v>
+      </c>
+      <c r="D127" t="s">
+        <v>1461</v>
+      </c>
+      <c r="E127" t="s">
+        <v>1412</v>
+      </c>
+      <c r="F127" t="s">
+        <v>1414</v>
+      </c>
+      <c r="G127" t="s">
+        <v>1415</v>
+      </c>
+      <c r="H127" t="s">
+        <v>1417</v>
+      </c>
+      <c r="I127" t="s">
+        <v>1419</v>
+      </c>
+      <c r="J127" t="s">
+        <v>1420</v>
+      </c>
+      <c r="K127" t="s">
+        <v>1422</v>
+      </c>
+      <c r="L127" t="s">
+        <v>1424</v>
+      </c>
+      <c r="M127" t="s">
+        <v>1426</v>
+      </c>
+      <c r="N127" t="s">
+        <v>1428</v>
+      </c>
+      <c r="O127" t="s">
+        <v>1430</v>
+      </c>
+      <c r="P127" t="s">
+        <v>1432</v>
+      </c>
+      <c r="Q127" t="s">
+        <v>1435</v>
+      </c>
+      <c r="R127" t="s">
+        <v>1438</v>
+      </c>
+    </row>
+    <row r="128" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>4</v>
+      </c>
+      <c r="B128" t="s">
+        <v>42</v>
+      </c>
+      <c r="C128" t="s">
+        <v>16</v>
+      </c>
+      <c r="D128" t="s">
+        <v>1405</v>
+      </c>
+      <c r="E128" t="s">
+        <v>1462</v>
+      </c>
+      <c r="F128" t="s">
+        <v>1463</v>
+      </c>
+      <c r="G128" s="75" t="s">
+        <v>1464</v>
+      </c>
+      <c r="H128" t="s">
+        <v>1465</v>
+      </c>
+      <c r="I128" s="49" t="s">
+        <v>1466</v>
+      </c>
+      <c r="J128" t="s">
+        <v>1467</v>
+      </c>
+      <c r="K128" t="s">
+        <v>1468</v>
+      </c>
+      <c r="L128" s="76" t="s">
+        <v>1469</v>
+      </c>
+      <c r="M128" s="77">
+        <v>2016</v>
+      </c>
+      <c r="N128" s="13" t="s">
+        <v>1470</v>
+      </c>
+      <c r="O128" s="14" t="s">
+        <v>1471</v>
+      </c>
+      <c r="P128" s="13">
+        <v>2016</v>
+      </c>
+      <c r="Q128" t="s">
+        <v>1434</v>
+      </c>
+      <c r="R128" t="s">
+        <v>1472</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>1406</v>
+      </c>
+      <c r="I130" s="49"/>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>14</v>
+      </c>
+      <c r="B131" t="s">
+        <v>40</v>
+      </c>
+      <c r="C131" t="s">
+        <v>15</v>
+      </c>
+      <c r="D131" t="s">
+        <v>1440</v>
+      </c>
+      <c r="E131" t="s">
+        <v>1473</v>
+      </c>
+      <c r="F131" t="s">
+        <v>1444</v>
+      </c>
+      <c r="G131" t="s">
+        <v>1474</v>
+      </c>
+      <c r="H131" t="s">
+        <v>622</v>
+      </c>
+      <c r="I131" s="49"/>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>4</v>
+      </c>
+      <c r="B132" t="s">
+        <v>42</v>
+      </c>
+      <c r="C132" t="s">
+        <v>16</v>
+      </c>
+      <c r="D132" t="s">
+        <v>1475</v>
+      </c>
+      <c r="E132" t="s">
+        <v>1475</v>
+      </c>
+      <c r="F132" s="78" t="s">
+        <v>1476</v>
+      </c>
+      <c r="G132" s="79" t="s">
+        <v>1477</v>
+      </c>
+      <c r="H132">
+        <v>12345678</v>
+      </c>
+      <c r="I132" s="49"/>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I133" s="49"/>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>1407</v>
+      </c>
+      <c r="I134" s="49"/>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>14</v>
+      </c>
+      <c r="B135" t="s">
+        <v>40</v>
+      </c>
+      <c r="C135" t="s">
+        <v>15</v>
+      </c>
+      <c r="D135" t="s">
+        <v>1440</v>
+      </c>
+      <c r="E135" t="s">
+        <v>1473</v>
+      </c>
+      <c r="F135" t="s">
+        <v>1444</v>
+      </c>
+      <c r="G135" t="s">
+        <v>1452</v>
+      </c>
+      <c r="H135" t="s">
+        <v>1453</v>
+      </c>
+      <c r="I135" s="49" t="s">
+        <v>1454</v>
+      </c>
+      <c r="J135" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A136" s="78" t="s">
+        <v>4</v>
+      </c>
+      <c r="B136" s="78" t="s">
+        <v>42</v>
+      </c>
+      <c r="C136" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="D136" s="78" t="s">
+        <v>1475</v>
+      </c>
+      <c r="E136" s="78" t="s">
+        <v>1475</v>
+      </c>
+      <c r="F136" s="78" t="s">
+        <v>1478</v>
+      </c>
+      <c r="G136" s="77" t="s">
+        <v>1479</v>
+      </c>
+      <c r="H136" s="78" t="s">
+        <v>1480</v>
+      </c>
+      <c r="I136" s="78" t="s">
+        <v>1481</v>
+      </c>
+      <c r="J136" s="78" t="s">
+        <v>1482</v>
       </c>
     </row>
   </sheetData>
@@ -27061,6 +28534,8 @@
     <hyperlink ref="T100" r:id="rId45" display="mailto:s.u.p.p.l.i.e.r.c.o.n.n.ection24@gmail.com"/>
     <hyperlink ref="Y104" r:id="rId46"/>
     <hyperlink ref="Y108" r:id="rId47"/>
+    <hyperlink ref="G128" r:id="rId48"/>
+    <hyperlink ref="G132" r:id="rId49"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>